<commit_message>
Sprint 8 - Limpeza
</commit_message>
<xml_diff>
--- a/Sprint 8/Sprint_8 Burndown-Backlog.xlsx
+++ b/Sprint 8/Sprint_8 Burndown-Backlog.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" tabRatio="990" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="96">
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
@@ -329,6 +329,9 @@
   <si>
     <t>Terça
 08/11/2016</t>
+  </si>
+  <si>
+    <t>Feito</t>
   </si>
 </sst>
 </file>
@@ -742,18 +745,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -766,10 +758,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -823,7 +827,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2808,28 +2811,28 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2941,31 +2944,31 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-7.75</c:v>
+                  <c:v>-3.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-13.75</c:v>
+                  <c:v>-9.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-17.95</c:v>
+                  <c:v>-13.95</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-24.95</c:v>
+                  <c:v>-20.95</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-32.700000000000003</c:v>
+                  <c:v>-28.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-38.200000000000003</c:v>
+                  <c:v>-34.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-45.7</c:v>
+                  <c:v>-41.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2993,11 +2996,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="164976656"/>
-        <c:axId val="165014464"/>
+        <c:axId val="189318040"/>
+        <c:axId val="189324304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="164976656"/>
+        <c:axId val="189318040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3078,7 +3081,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165014464"/>
+        <c:crossAx val="189324304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3086,7 +3089,509 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165014464"/>
+        <c:axId val="189324304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>TEMPO EM HORAS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47520">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="189318040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Diogo!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25560">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Diogo!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>(hrs)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Terça
+01/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Quarta
+02/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quinta
+03/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sexta
+04/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sábado
+05/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Domingo
+06/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Segunda
+07/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Terça
+08/11/2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Diogo!$B$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4415-482B-ACC6-22BD17151AFA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Diogo!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25560">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Diogo!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>(hrs)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Terça
+01/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Quarta
+02/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quinta
+03/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sexta
+04/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sábado
+05/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Domingo
+06/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Segunda
+07/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Terça
+08/11/2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Diogo!$B$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4415-482B-ACC6-22BD17151AFA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="189402944"/>
+        <c:axId val="189403328"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="189402944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>DIAS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="222222"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="189403328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="189403328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3169,511 +3674,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164976656"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:noFill/>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Diogo!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25560">
-              <a:solidFill>
-                <a:srgbClr val="0000FF"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Diogo!$B$3:$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>(hrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Terça
-01/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Quarta
-02/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Quinta
-03/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sexta
-04/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sábado
-05/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Domingo
-06/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Segunda
-07/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Terça
-08/11/2016</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Diogo!$B$5:$J$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4415-482B-ACC6-22BD17151AFA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Diogo!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25560">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Diogo!$B$3:$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>(hrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Terça
-01/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Quarta
-02/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Quinta
-03/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sexta
-04/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sábado
-05/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Domingo
-06/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Segunda
-07/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Terça
-08/11/2016</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Diogo!$B$6:$J$6</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4415-482B-ACC6-22BD17151AFA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="164565576"/>
-        <c:axId val="164565960"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="164565576"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>DIAS</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="222222"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="164565960"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="164565960"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>TEMPO EM HORAS</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47520">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="164565576"/>
+        <c:crossAx val="189402944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4008,11 +4009,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="165103760"/>
-        <c:axId val="165780688"/>
+        <c:axId val="189529928"/>
+        <c:axId val="189530312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="165103760"/>
+        <c:axId val="189529928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4054,7 +4055,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4086,7 +4086,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165780688"/>
+        <c:crossAx val="189530312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4094,7 +4094,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165780688"/>
+        <c:axId val="189530312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4145,7 +4145,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4177,7 +4176,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165103760"/>
+        <c:crossAx val="189529928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4190,7 +4189,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4512,11 +4510,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="165755544"/>
-        <c:axId val="165755928"/>
+        <c:axId val="189469168"/>
+        <c:axId val="191118864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="165755544"/>
+        <c:axId val="189469168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4558,7 +4556,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4590,7 +4587,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165755928"/>
+        <c:crossAx val="191118864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4598,7 +4595,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165755928"/>
+        <c:axId val="191118864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4649,7 +4646,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4681,7 +4677,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165755544"/>
+        <c:crossAx val="189469168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4694,7 +4690,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5163,8 +5158,8 @@
   </sheetPr>
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5181,16 +5176,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5215,27 +5210,27 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34" t="s">
+      <c r="G2" s="41"/>
+      <c r="H2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="34">
+      <c r="I2" s="41">
         <v>8</v>
       </c>
       <c r="J2" s="3"/>
@@ -5259,9 +5254,9 @@
       <c r="AB2" s="4"/>
     </row>
     <row r="3" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -5274,8 +5269,8 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -5297,25 +5292,31 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="42" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="41">
+      <c r="C4" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="25">
+        <v>1</v>
+      </c>
+      <c r="E4" s="38">
         <f>SUM(D4:D6)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="41">
+        <v>4</v>
+      </c>
+      <c r="F4" s="25">
+        <v>1</v>
+      </c>
+      <c r="G4" s="38">
         <f>SUM(F4:F6)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="I4" s="29"/>
       <c r="J4" s="31"/>
@@ -5339,17 +5340,23 @@
       <c r="AB4" s="4"/>
     </row>
     <row r="5" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="43"/>
+      <c r="C5" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="25">
+        <v>1</v>
+      </c>
+      <c r="E5" s="39"/>
+      <c r="F5" s="25">
+        <v>1</v>
+      </c>
+      <c r="G5" s="39"/>
       <c r="H5" s="32" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="3"/>
@@ -5373,17 +5380,23 @@
       <c r="AB5" s="4"/>
     </row>
     <row r="6" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="42"/>
+      <c r="C6" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="27">
+        <v>2</v>
+      </c>
+      <c r="E6" s="40"/>
+      <c r="F6" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="40"/>
       <c r="H6" s="32" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="3"/>
@@ -5407,7 +5420,7 @@
       <c r="AB6" s="4"/>
     </row>
     <row r="7" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="35" t="s">
         <v>73</v>
       </c>
       <c r="B7" s="22" t="s">
@@ -5415,12 +5428,12 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="28"/>
-      <c r="E7" s="41">
+      <c r="E7" s="38">
         <f>SUM(D7:D11)</f>
         <v>0</v>
       </c>
       <c r="F7" s="28"/>
-      <c r="G7" s="41">
+      <c r="G7" s="38">
         <f>SUM(F7:F11)</f>
         <v>0</v>
       </c>
@@ -5447,15 +5460,15 @@
       <c r="AB7" s="4"/>
     </row>
     <row r="8" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="22" t="s">
         <v>83</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
-      <c r="E8" s="43"/>
+      <c r="E8" s="39"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="43"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="32" t="s">
         <v>67</v>
       </c>
@@ -5479,15 +5492,15 @@
       <c r="AB8" s="4"/>
     </row>
     <row r="9" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="39"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="23" t="s">
         <v>85</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="43"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="20"/>
-      <c r="G9" s="43"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="32" t="s">
         <v>67</v>
       </c>
@@ -5512,15 +5525,15 @@
       <c r="AB9" s="4"/>
     </row>
     <row r="10" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="39"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="24" t="s">
         <v>87</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
-      <c r="E10" s="43"/>
+      <c r="E10" s="39"/>
       <c r="F10" s="20"/>
-      <c r="G10" s="43"/>
+      <c r="G10" s="39"/>
       <c r="H10" s="32" t="s">
         <v>67</v>
       </c>
@@ -5545,15 +5558,15 @@
       <c r="AB10" s="4"/>
     </row>
     <row r="11" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="23" t="s">
         <v>86</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
-      <c r="E11" s="42"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="20"/>
-      <c r="G11" s="42"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="32" t="s">
         <v>67</v>
       </c>
@@ -5578,20 +5591,20 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="34" t="s">
         <v>68</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
-      <c r="E12" s="41">
+      <c r="E12" s="38">
         <f>SUM(D12:D21)</f>
         <v>0</v>
       </c>
       <c r="F12" s="20"/>
-      <c r="G12" s="41">
+      <c r="G12" s="38">
         <f>SUM(F12:F21)</f>
         <v>0</v>
       </c>
@@ -5619,15 +5632,15 @@
       <c r="AB12" s="4"/>
     </row>
     <row r="13" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="39"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
-      <c r="E13" s="43"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="20"/>
-      <c r="G13" s="43"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="32" t="s">
         <v>67</v>
       </c>
@@ -5652,15 +5665,15 @@
       <c r="AB13" s="4"/>
     </row>
     <row r="14" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="39"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="22" t="s">
         <v>74</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
-      <c r="E14" s="43"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="20"/>
-      <c r="G14" s="43"/>
+      <c r="G14" s="39"/>
       <c r="H14" s="32" t="s">
         <v>67</v>
       </c>
@@ -5685,15 +5698,15 @@
       <c r="AB14" s="4"/>
     </row>
     <row r="15" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="22" t="s">
         <v>75</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
-      <c r="E15" s="43"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="20"/>
-      <c r="G15" s="43"/>
+      <c r="G15" s="39"/>
       <c r="H15" s="32" t="s">
         <v>67</v>
       </c>
@@ -5718,15 +5731,15 @@
       <c r="AB15" s="4"/>
     </row>
     <row r="16" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="39"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="22" t="s">
         <v>76</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
-      <c r="E16" s="43"/>
+      <c r="E16" s="39"/>
       <c r="F16" s="20"/>
-      <c r="G16" s="43"/>
+      <c r="G16" s="39"/>
       <c r="H16" s="32" t="s">
         <v>67</v>
       </c>
@@ -5751,15 +5764,15 @@
       <c r="AB16" s="4"/>
     </row>
     <row r="17" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="39"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="22" t="s">
         <v>77</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
-      <c r="E17" s="43"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="20"/>
-      <c r="G17" s="43"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="32" t="s">
         <v>67</v>
       </c>
@@ -5784,15 +5797,15 @@
       <c r="AB17" s="4"/>
     </row>
     <row r="18" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="22" t="s">
         <v>78</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
-      <c r="E18" s="43"/>
+      <c r="E18" s="39"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="43"/>
+      <c r="G18" s="39"/>
       <c r="H18" s="32" t="s">
         <v>67</v>
       </c>
@@ -5817,15 +5830,15 @@
       <c r="AB18" s="4"/>
     </row>
     <row r="19" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="39"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="22" t="s">
         <v>79</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
-      <c r="E19" s="43"/>
+      <c r="E19" s="39"/>
       <c r="F19" s="20"/>
-      <c r="G19" s="43"/>
+      <c r="G19" s="39"/>
       <c r="H19" s="32" t="s">
         <v>67</v>
       </c>
@@ -5850,15 +5863,15 @@
       <c r="AB19" s="4"/>
     </row>
     <row r="20" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="39"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="22" t="s">
         <v>80</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="43"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="20"/>
-      <c r="G20" s="43"/>
+      <c r="G20" s="39"/>
       <c r="H20" s="32" t="s">
         <v>67</v>
       </c>
@@ -5883,15 +5896,15 @@
       <c r="AB20" s="4"/>
     </row>
     <row r="21" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="39"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="22" t="s">
         <v>81</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
-      <c r="E21" s="43"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="20"/>
-      <c r="G21" s="43"/>
+      <c r="G21" s="39"/>
       <c r="H21" s="32" t="s">
         <v>67</v>
       </c>
@@ -5916,7 +5929,7 @@
       <c r="AB21" s="4"/>
     </row>
     <row r="22" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="35" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="26" t="s">
@@ -5924,12 +5937,12 @@
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
-      <c r="E22" s="41">
+      <c r="E22" s="38">
         <f>SUM(D22:D24)</f>
         <v>0</v>
       </c>
       <c r="F22" s="20"/>
-      <c r="G22" s="41">
+      <c r="G22" s="38">
         <f>SUM(F22:F24)</f>
         <v>0</v>
       </c>
@@ -5950,15 +5963,15 @@
       <c r="T22" s="4"/>
     </row>
     <row r="23" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="39"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="21" t="s">
         <v>54</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
-      <c r="E23" s="43"/>
+      <c r="E23" s="39"/>
       <c r="F23" s="20"/>
-      <c r="G23" s="43"/>
+      <c r="G23" s="39"/>
       <c r="H23" s="32" t="s">
         <v>67</v>
       </c>
@@ -5976,15 +5989,15 @@
       <c r="T23" s="4"/>
     </row>
     <row r="24" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="40"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
-      <c r="E24" s="42"/>
+      <c r="E24" s="40"/>
       <c r="F24" s="20"/>
-      <c r="G24" s="42"/>
+      <c r="G24" s="40"/>
       <c r="H24" s="32" t="s">
         <v>67</v>
       </c>
@@ -6192,6 +6205,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G4:G6"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="E22:E24"/>
     <mergeCell ref="G22:G24"/>
@@ -6205,13 +6225,6 @@
     <mergeCell ref="G12:G21"/>
     <mergeCell ref="A12:A21"/>
     <mergeCell ref="E12:E21"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G4:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:I6">
     <cfRule type="expression" dxfId="127" priority="2">
@@ -6256,20 +6269,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -6328,40 +6341,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="47">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="48" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -6373,18 +6386,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -6399,35 +6412,35 @@
       </c>
       <c r="B5" s="12">
         <f>SUM('Sprint Backlog'!D:D)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="13">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="D5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J5" s="13">
         <f t="shared" si="1"/>
@@ -6435,11 +6448,11 @@
       </c>
       <c r="K5" s="13">
         <f>SUM(C5:J5)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L5" s="13">
         <f>K5/A$3</f>
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -6455,47 +6468,47 @@
       </c>
       <c r="B6" s="12">
         <f>B5</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C6" s="13">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6" s="13">
         <f t="shared" si="2"/>
-        <v>-7.75</v>
+        <v>-3.75</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" si="2"/>
-        <v>-13.75</v>
+        <v>-9.75</v>
       </c>
       <c r="F6" s="13">
         <f t="shared" si="2"/>
-        <v>-17.95</v>
+        <v>-13.95</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" si="2"/>
-        <v>-24.95</v>
+        <v>-20.95</v>
       </c>
       <c r="H6" s="13">
         <f t="shared" si="2"/>
-        <v>-32.700000000000003</v>
+        <v>-28.7</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" si="2"/>
-        <v>-38.200000000000003</v>
+        <v>-34.200000000000003</v>
       </c>
       <c r="J6" s="13">
         <f t="shared" si="2"/>
-        <v>-45.7</v>
+        <v>-41.7</v>
       </c>
       <c r="K6" s="13">
         <f>SUM(C6:J6)</f>
-        <v>-181</v>
+        <v>-149</v>
       </c>
       <c r="L6" s="13">
         <f>K6/A$3</f>
-        <v>-22.625</v>
+        <v>-18.625</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -6533,18 +6546,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -6559,7 +6572,7 @@
       </c>
       <c r="B9" s="16">
         <f>B5/A3</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C9" s="16">
         <f t="shared" ref="C9:K9" si="3">SUM(C10:C12)</f>
@@ -6615,7 +6628,7 @@
       </c>
       <c r="B10" s="18">
         <f>Diogo!B9</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C10" s="13">
         <f>Diogo!C9</f>
@@ -7268,7 +7281,7 @@
   </sheetPr>
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
@@ -7284,20 +7297,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -7356,40 +7369,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="47">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="48" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -7401,18 +7414,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -7427,35 +7440,35 @@
       </c>
       <c r="B5" s="12">
         <f>SUMIF('Sprint Backlog'!C:C,"=Diogo",'Sprint Backlog'!D:D)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="13">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="D5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J5" s="13">
         <f t="shared" si="1"/>
@@ -7463,11 +7476,11 @@
       </c>
       <c r="K5" s="13">
         <f>SUM(C5:J5)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L5" s="13">
         <f>K5/A$3</f>
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -7483,47 +7496,47 @@
       </c>
       <c r="B6" s="12">
         <f>B5</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C6" s="13">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K6" s="13">
         <f>SUM(C6:J6)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="L6" s="13">
         <f>K6/A$3</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -7561,18 +7574,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -7587,7 +7600,7 @@
       </c>
       <c r="B9" s="16">
         <f>B5/A3</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C9" s="16">
         <f t="shared" ref="C9:L9" si="3">SUM(C10:C12)</f>
@@ -7638,10 +7651,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="54"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="13">
         <v>0</v>
       </c>
@@ -7675,18 +7688,18 @@
         <v>0</v>
       </c>
       <c r="M10" s="7"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="52"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="13">
         <v>0</v>
       </c>
@@ -7720,18 +7733,18 @@
         <v>0</v>
       </c>
       <c r="M11" s="7"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="52"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="53"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="52"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="13">
         <v>0</v>
       </c>
@@ -7765,18 +7778,18 @@
         <v>0</v>
       </c>
       <c r="M12" s="7"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="53"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="52"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="13">
         <v>0</v>
       </c>
@@ -7818,10 +7831,10 @@
       <c r="S13" s="7"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="52"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="13">
         <v>0</v>
       </c>
@@ -7863,10 +7876,10 @@
       <c r="S14" s="7"/>
     </row>
     <row r="15" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="52"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="13">
         <v>0</v>
       </c>
@@ -7908,10 +7921,10 @@
       <c r="S15" s="7"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="52"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="13">
         <v>0</v>
       </c>
@@ -7953,10 +7966,10 @@
       <c r="S16" s="7"/>
     </row>
     <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="52"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="13">
         <v>0</v>
       </c>
@@ -7998,10 +8011,10 @@
       <c r="S17" s="7"/>
     </row>
     <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="52"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="13">
         <v>0</v>
       </c>
@@ -8043,10 +8056,10 @@
       <c r="S18" s="7"/>
     </row>
     <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="52"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="13">
         <v>0</v>
       </c>
@@ -8118,6 +8131,18 @@
     <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
@@ -8134,18 +8159,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <conditionalFormatting sqref="N10:O19 N21:O22 L20:M20 C21:L102 A20:J20 C10:L19">
     <cfRule type="expression" dxfId="29" priority="2">
@@ -8199,20 +8212,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -8271,40 +8284,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="47">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="48" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -8316,18 +8329,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -8476,18 +8489,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -8553,10 +8566,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="54"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="13">
         <v>0</v>
       </c>
@@ -8598,10 +8611,10 @@
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="54"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="13">
         <v>0</v>
       </c>
@@ -8643,10 +8656,10 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="13">
         <v>0</v>
       </c>
@@ -8688,10 +8701,10 @@
       <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="60"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="13">
         <v>0</v>
       </c>
@@ -8726,10 +8739,10 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="56"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="13">
         <v>0</v>
       </c>
@@ -8764,10 +8777,10 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="56"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="13">
         <v>0</v>
       </c>
@@ -8802,10 +8815,10 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="56"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="13">
         <v>0</v>
       </c>
@@ -8840,10 +8853,10 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="13">
         <v>0</v>
       </c>
@@ -8881,6 +8894,14 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
@@ -8896,14 +8917,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:L98 K10:L10 A14:A17">
     <cfRule type="expression" dxfId="24" priority="17">
@@ -9003,20 +9016,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -9075,40 +9088,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="47">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="48" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -9120,18 +9133,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -9280,18 +9293,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -9357,10 +9370,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="54"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="13">
         <v>0</v>
       </c>
@@ -9402,10 +9415,10 @@
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="54"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="13">
         <v>0</v>
       </c>
@@ -9447,10 +9460,10 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="54"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="13">
         <v>0</v>
       </c>
@@ -9492,10 +9505,10 @@
       <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="56"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="13">
         <v>0</v>
       </c>
@@ -9530,10 +9543,10 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="56"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="13">
         <v>0</v>
       </c>
@@ -9559,7 +9572,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="13">
-        <f t="shared" ref="K14:K17" si="4">SUM(C14:J14)</f>
+        <f t="shared" ref="K14:K16" si="4">SUM(C14:J14)</f>
         <v>0</v>
       </c>
       <c r="L14" s="13">
@@ -9568,10 +9581,10 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="56"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="13">
         <v>0</v>
       </c>
@@ -9606,10 +9619,10 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="56"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="13">
         <v>0</v>
       </c>
@@ -9644,10 +9657,10 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="13">
         <v>0</v>
       </c>
@@ -9686,6 +9699,14 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C1:L1"/>
@@ -9701,14 +9722,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:L96">
     <cfRule type="expression" dxfId="9" priority="19">

</xml_diff>

<commit_message>
Métodos cad e cons de Pac e Func
</commit_message>
<xml_diff>
--- a/Sprint 8/Sprint_8 Burndown-Backlog.xlsx
+++ b/Sprint 8/Sprint_8 Burndown-Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izaquiel\Desktop\PDS\Sprint 8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izaquiel\Desktop\projetoPdsTeste\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="110">
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
@@ -344,6 +344,36 @@
   </si>
   <si>
     <t>Criação de script para esquema do banco de dados</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de alteração de paciente</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de alteração de funcionário</t>
+  </si>
+  <si>
+    <t>Criação de método cadastro de paciente</t>
+  </si>
+  <si>
+    <t>Criação de método consulta de paciente</t>
+  </si>
+  <si>
+    <t>Criação de método alteração de paciente</t>
+  </si>
+  <si>
+    <t>Criação de método cadastro de funcionário</t>
+  </si>
+  <si>
+    <t>Criação de método consulta de funcionario</t>
+  </si>
+  <si>
+    <t>Criação de método alteração de funcionário</t>
+  </si>
+  <si>
+    <t>Teste de inserção e consulta de funcionario</t>
+  </si>
+  <si>
+    <t>Teste de inserção e consulta de paciente</t>
   </si>
 </sst>
 </file>
@@ -744,6 +774,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -760,18 +802,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2803,28 +2833,28 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>20</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.5</c:v>
+                  <c:v>23.1875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>19.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.5</c:v>
+                  <c:v>16.5625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>13.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.5</c:v>
+                  <c:v>9.9375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>6.625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5</c:v>
+                  <c:v>3.3125</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2936,31 +2966,31 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>20</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.25</c:v>
+                  <c:v>18.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.25</c:v>
+                  <c:v>12.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0499999999999998</c:v>
+                  <c:v>8.5500000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.95</c:v>
+                  <c:v>1.5500000000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-12.7</c:v>
+                  <c:v>-6.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-18.2</c:v>
+                  <c:v>-11.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-25.7</c:v>
+                  <c:v>-19.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2988,11 +3018,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="133809104"/>
-        <c:axId val="133808712"/>
+        <c:axId val="171664408"/>
+        <c:axId val="171665976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133809104"/>
+        <c:axId val="171664408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3073,7 +3103,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133808712"/>
+        <c:crossAx val="171665976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3081,7 +3111,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133808712"/>
+        <c:axId val="171665976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3163,7 +3193,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133809104"/>
+        <c:crossAx val="171664408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3497,1019 +3527,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="133809496"/>
-        <c:axId val="133809888"/>
+        <c:axId val="171666760"/>
+        <c:axId val="171663232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133809496"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>DIAS</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="222222"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="133809888"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="133809888"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>TEMPO EM HORAS</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47520">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="133809496"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:noFill/>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Izaquiel!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25560">
-              <a:solidFill>
-                <a:srgbClr val="0000FF"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Izaquiel!$B$3:$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>(hrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Terça
-25/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Quarta
-26/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Quinta
-27/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sexta
-28/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sábado
-29/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Domingo
-30/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Segunda
-31/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Terça
-25/10/2016</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Izaquiel!$B$5:$J$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5DC1-45E4-B87A-C4BF8E3DF284}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Izaquiel!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25560">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Izaquiel!$B$3:$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>(hrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Terça
-25/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Quarta
-26/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Quinta
-27/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sexta
-28/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sábado
-29/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Domingo
-30/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Segunda
-31/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Terça
-25/10/2016</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Izaquiel!$B$6:$J$6</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5DC1-45E4-B87A-C4BF8E3DF284}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="177580512"/>
-        <c:axId val="177584824"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="177580512"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>DIAS</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="222222"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="177584824"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="177584824"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>TEMPO EM HORAS</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47520">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="177580512"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:noFill/>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ivo!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25560">
-              <a:solidFill>
-                <a:srgbClr val="0000FF"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Ivo!$B$3:$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>(hrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Terça
-01/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Quarta
-02/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Quinta
-03/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sexta
-04/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sábado
-05/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Domingo
-06/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Segunda
-07/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Terça
-08/11/2016</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Ivo!$B$5:$J$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1ED5-4BB2-A00B-9F8936EBC51C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ivo!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25560">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Ivo!$B$3:$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>(hrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Terça
-01/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Quarta
-02/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Quinta
-03/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sexta
-04/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sábado
-05/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Domingo
-06/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Segunda
-07/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Terça
-08/11/2016</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Ivo!$B$6:$J$6</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1ED5-4BB2-A00B-9F8936EBC51C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="177585216"/>
-        <c:axId val="177583256"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="177585216"/>
+        <c:axId val="171666760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4582,7 +3604,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177583256"/>
+        <c:crossAx val="171663232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4590,7 +3612,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="177583256"/>
+        <c:axId val="171663232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4672,7 +3694,1009 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177585216"/>
+        <c:crossAx val="171666760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Izaquiel!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25560">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Izaquiel!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>(hrs)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Terça
+25/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Quarta
+26/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quinta
+27/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sexta
+28/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sábado
+29/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Domingo
+30/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Segunda
+31/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Terça
+25/10/2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Izaquiel!$B$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.8125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5DC1-45E4-B87A-C4BF8E3DF284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Izaquiel!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25560">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Izaquiel!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>(hrs)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Terça
+25/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Quarta
+26/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quinta
+27/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sexta
+28/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sábado
+29/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Domingo
+30/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Segunda
+31/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Terça
+25/10/2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Izaquiel!$B$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5DC1-45E4-B87A-C4BF8E3DF284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="173612960"/>
+        <c:axId val="173613352"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="173612960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>DIAS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="222222"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="173613352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="173613352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>TEMPO EM HORAS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47520">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="173612960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Ivo!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25560">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Ivo!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>(hrs)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Terça
+01/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Quarta
+02/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quinta
+03/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sexta
+04/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sábado
+05/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Domingo
+06/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Segunda
+07/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Terça
+08/11/2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Ivo!$B$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1ED5-4BB2-A00B-9F8936EBC51C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Ivo!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25560">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Ivo!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>(hrs)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Terça
+01/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Quarta
+02/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quinta
+03/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sexta
+04/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sábado
+05/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Domingo
+06/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Segunda
+07/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Terça
+08/11/2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Ivo!$B$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1ED5-4BB2-A00B-9F8936EBC51C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="173610608"/>
+        <c:axId val="173609824"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="173610608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>DIAS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="222222"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="173609824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="173609824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>TEMPO EM HORAS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47520">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="173610608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5151,10 +5175,10 @@
   <sheetPr>
     <tabColor rgb="FF38761D"/>
   </sheetPr>
-  <dimension ref="A1:AB37"/>
+  <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5171,16 +5195,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5205,27 +5229,27 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="40">
+      <c r="I2" s="34">
         <v>8</v>
       </c>
       <c r="J2" s="3"/>
@@ -5249,9 +5273,9 @@
       <c r="AB2" s="4"/>
     </row>
     <row r="3" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -5264,8 +5288,8 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -5287,7 +5311,7 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="35" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="25" t="s">
@@ -5299,14 +5323,14 @@
       <c r="D4" s="24">
         <v>1</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="41">
         <f>SUM(D4:D6)</f>
         <v>4</v>
       </c>
       <c r="F4" s="24">
         <v>1</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="41">
         <f>SUM(F4:F6)</f>
         <v>3.5</v>
       </c>
@@ -5335,7 +5359,7 @@
       <c r="AB4" s="4"/>
     </row>
     <row r="5" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="20" t="s">
         <v>84</v>
       </c>
@@ -5345,11 +5369,11 @@
       <c r="D5" s="24">
         <v>1</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="42"/>
       <c r="F5" s="24">
         <v>1</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="31" t="s">
         <v>95</v>
       </c>
@@ -5375,7 +5399,7 @@
       <c r="AB5" s="4"/>
     </row>
     <row r="6" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="43"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="21" t="s">
         <v>72</v>
       </c>
@@ -5385,11 +5409,11 @@
       <c r="D6" s="26">
         <v>2</v>
       </c>
-      <c r="E6" s="39"/>
+      <c r="E6" s="43"/>
       <c r="F6" s="26">
         <v>1.5</v>
       </c>
-      <c r="G6" s="39"/>
+      <c r="G6" s="43"/>
       <c r="H6" s="31" t="s">
         <v>95</v>
       </c>
@@ -5415,7 +5439,7 @@
       <c r="AB6" s="4"/>
     </row>
     <row r="7" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="38" t="s">
         <v>73</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -5427,14 +5451,14 @@
       <c r="D7" s="27">
         <v>2</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="41">
         <f>SUM(D7:D11)</f>
         <v>10</v>
       </c>
       <c r="F7" s="27">
         <v>2</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="41">
         <f>SUM(F7:F11)</f>
         <v>8.5</v>
       </c>
@@ -5461,7 +5485,7 @@
       <c r="AB7" s="4"/>
     </row>
     <row r="8" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="21" t="s">
         <v>83</v>
       </c>
@@ -5471,11 +5495,11 @@
       <c r="D8" s="19">
         <v>2</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="19">
         <v>1.5</v>
       </c>
-      <c r="G8" s="38"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="31" t="s">
         <v>95</v>
       </c>
@@ -5499,7 +5523,7 @@
       <c r="AB8" s="4"/>
     </row>
     <row r="9" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="22" t="s">
         <v>85</v>
       </c>
@@ -5509,11 +5533,11 @@
       <c r="D9" s="19">
         <v>1</v>
       </c>
-      <c r="E9" s="38"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="19">
         <v>1</v>
       </c>
-      <c r="G9" s="38"/>
+      <c r="G9" s="42"/>
       <c r="H9" s="31" t="s">
         <v>95</v>
       </c>
@@ -5538,7 +5562,7 @@
       <c r="AB9" s="4"/>
     </row>
     <row r="10" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="35"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="23" t="s">
         <v>87</v>
       </c>
@@ -5548,11 +5572,11 @@
       <c r="D10" s="19">
         <v>3</v>
       </c>
-      <c r="E10" s="38"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="19">
         <v>2.5</v>
       </c>
-      <c r="G10" s="38"/>
+      <c r="G10" s="42"/>
       <c r="H10" s="31" t="s">
         <v>95</v>
       </c>
@@ -5577,7 +5601,7 @@
       <c r="AB10" s="4"/>
     </row>
     <row r="11" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="22" t="s">
         <v>86</v>
       </c>
@@ -5587,11 +5611,11 @@
       <c r="D11" s="19">
         <v>2</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="19">
         <v>1.5</v>
       </c>
-      <c r="G11" s="39"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="31" t="s">
         <v>95</v>
       </c>
@@ -5616,7 +5640,7 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="38" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -5628,16 +5652,16 @@
       <c r="D12" s="19">
         <v>2</v>
       </c>
-      <c r="E12" s="37">
-        <f>SUM(D12:D25)</f>
-        <v>6</v>
+      <c r="E12" s="41">
+        <f>SUM(D12:D35)</f>
+        <v>12.5</v>
       </c>
       <c r="F12" s="19">
         <v>1.25</v>
       </c>
-      <c r="G12" s="37">
-        <f>SUM(F12:F25)</f>
-        <v>4.75</v>
+      <c r="G12" s="41">
+        <f>SUM(F12:F35)</f>
+        <v>9.75</v>
       </c>
       <c r="H12" s="31" t="s">
         <v>95</v>
@@ -5663,7 +5687,7 @@
       <c r="AB12" s="4"/>
     </row>
     <row r="13" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="23" t="s">
         <v>96</v>
       </c>
@@ -5673,11 +5697,11 @@
       <c r="D13" s="19">
         <v>2</v>
       </c>
-      <c r="E13" s="38"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="19">
         <v>1.5</v>
       </c>
-      <c r="G13" s="38"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="31" t="s">
         <v>95</v>
       </c>
@@ -5702,7 +5726,7 @@
       <c r="AB13" s="4"/>
     </row>
     <row r="14" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="23" t="s">
         <v>98</v>
       </c>
@@ -5712,11 +5736,11 @@
       <c r="D14" s="19">
         <v>1</v>
       </c>
-      <c r="E14" s="38"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="19">
         <v>1</v>
       </c>
-      <c r="G14" s="38"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="31" t="s">
         <v>95</v>
       </c>
@@ -5741,7 +5765,7 @@
       <c r="AB14" s="4"/>
     </row>
     <row r="15" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="23" t="s">
         <v>99</v>
       </c>
@@ -5751,11 +5775,11 @@
       <c r="D15" s="19">
         <v>1</v>
       </c>
-      <c r="E15" s="38"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="19">
         <v>1</v>
       </c>
-      <c r="G15" s="38"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="31" t="s">
         <v>95</v>
       </c>
@@ -5780,15 +5804,15 @@
       <c r="AB15" s="4"/>
     </row>
     <row r="16" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="35"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="33" t="s">
         <v>68</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="38"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="19"/>
-      <c r="G16" s="38"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="31" t="s">
         <v>67</v>
       </c>
@@ -5813,15 +5837,15 @@
       <c r="AB16" s="4"/>
     </row>
     <row r="17" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="23" t="s">
         <v>69</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="38"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="38"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="31" t="s">
         <v>67</v>
       </c>
@@ -5846,17 +5870,23 @@
       <c r="AB17" s="4"/>
     </row>
     <row r="18" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="35"/>
-      <c r="B18" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="38"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="19">
+        <v>1</v>
+      </c>
+      <c r="E18" s="42"/>
+      <c r="F18" s="19">
+        <v>1</v>
+      </c>
+      <c r="G18" s="42"/>
       <c r="H18" s="31" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="I18" s="5"/>
       <c r="K18" s="4"/>
@@ -5879,17 +5909,23 @@
       <c r="AB18" s="4"/>
     </row>
     <row r="19" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="35"/>
-      <c r="B19" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="38"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="42"/>
+      <c r="F19" s="19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="42"/>
       <c r="H19" s="31" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="I19" s="5"/>
       <c r="K19" s="4"/>
@@ -5912,17 +5948,23 @@
       <c r="AB19" s="4"/>
     </row>
     <row r="20" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="35"/>
-      <c r="B20" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="19">
+        <v>1</v>
+      </c>
+      <c r="E20" s="42"/>
+      <c r="F20" s="19">
+        <v>1</v>
+      </c>
+      <c r="G20" s="42"/>
       <c r="H20" s="31" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="I20" s="5"/>
       <c r="K20" s="4"/>
@@ -5945,17 +5987,23 @@
       <c r="AB20" s="4"/>
     </row>
     <row r="21" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="35"/>
-      <c r="B21" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="38"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="E21" s="42"/>
+      <c r="F21" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="G21" s="42"/>
       <c r="H21" s="31" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="I21" s="5"/>
       <c r="K21" s="4"/>
@@ -5978,17 +6026,23 @@
       <c r="AB21" s="4"/>
     </row>
     <row r="22" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="35"/>
-      <c r="B22" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="38"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="19">
+        <v>1</v>
+      </c>
+      <c r="E22" s="42"/>
+      <c r="F22" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="42"/>
       <c r="H22" s="31" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="I22" s="5"/>
       <c r="K22" s="4"/>
@@ -6011,17 +6065,23 @@
       <c r="AB22" s="4"/>
     </row>
     <row r="23" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="35"/>
-      <c r="B23" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="38"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="19">
+        <v>1</v>
+      </c>
+      <c r="E23" s="42"/>
+      <c r="F23" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="42"/>
       <c r="H23" s="31" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="I23" s="5"/>
       <c r="K23" s="4"/>
@@ -6044,17 +6104,23 @@
       <c r="AB23" s="4"/>
     </row>
     <row r="24" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="35"/>
-      <c r="B24" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="38"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="19">
+        <v>1</v>
+      </c>
+      <c r="E24" s="42"/>
+      <c r="F24" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="42"/>
       <c r="H24" s="31" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="I24" s="5"/>
       <c r="K24" s="4"/>
@@ -6077,17 +6143,23 @@
       <c r="AB24" s="4"/>
     </row>
     <row r="25" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
-      <c r="B25" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="39"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="E25" s="42"/>
+      <c r="F25" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="G25" s="42"/>
       <c r="H25" s="31" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="I25" s="5"/>
       <c r="K25" s="4"/>
@@ -6110,28 +6182,19 @@
       <c r="AB25" s="4"/>
     </row>
     <row r="26" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>53</v>
+      <c r="A26" s="39"/>
+      <c r="B26" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
-      <c r="E26" s="37">
-        <f>SUM(D26:D28)</f>
-        <v>0</v>
-      </c>
+      <c r="E26" s="42"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="37">
-        <f>SUM(F26:F28)</f>
-        <v>0</v>
-      </c>
+      <c r="G26" s="42"/>
       <c r="H26" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="I26" s="5"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -6142,22 +6205,29 @@
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
     </row>
     <row r="27" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="35"/>
-      <c r="B27" s="20" t="s">
-        <v>54</v>
+      <c r="A27" s="39"/>
+      <c r="B27" s="21" t="s">
+        <v>75</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
-      <c r="E27" s="38"/>
+      <c r="E27" s="42"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="38"/>
+      <c r="G27" s="42"/>
       <c r="H27" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="I27" s="5"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -6168,22 +6238,29 @@
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
     </row>
     <row r="28" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="36"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="21" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
-      <c r="E28" s="39"/>
+      <c r="E28" s="42"/>
       <c r="F28" s="19"/>
-      <c r="G28" s="39"/>
+      <c r="G28" s="42"/>
       <c r="H28" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="I28" s="5"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -6194,17 +6271,29 @@
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
     </row>
     <row r="29" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="5"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
@@ -6215,17 +6304,29 @@
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
-    </row>
-    <row r="30" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+    </row>
+    <row r="30" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="39"/>
+      <c r="B30" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I30" s="5"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -6236,17 +6337,29 @@
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
     </row>
     <row r="31" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I31" s="5"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -6257,16 +6370,29 @@
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
       <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4"/>
+      <c r="AB31" s="4"/>
     </row>
     <row r="32" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I32" s="5"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
@@ -6277,16 +6403,29 @@
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
       <c r="T32" s="4"/>
-    </row>
-    <row r="33" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4"/>
+      <c r="AA32" s="4"/>
+      <c r="AB32" s="4"/>
+    </row>
+    <row r="33" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="39"/>
+      <c r="B33" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I33" s="5"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -6297,16 +6436,29 @@
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
-    </row>
-    <row r="34" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="4"/>
+      <c r="AB33" s="4"/>
+    </row>
+    <row r="34" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="39"/>
+      <c r="B34" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I34" s="5"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -6317,18 +6469,29 @@
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
       <c r="T34" s="4"/>
-    </row>
-    <row r="35" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="4"/>
+      <c r="AB34" s="4"/>
+    </row>
+    <row r="35" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A35" s="40"/>
+      <c r="B35" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I35" s="5"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -6339,16 +6502,36 @@
       <c r="R35" s="4"/>
       <c r="S35" s="4"/>
       <c r="T35" s="4"/>
-    </row>
-    <row r="36" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4"/>
+      <c r="AA35" s="4"/>
+      <c r="AB35" s="4"/>
+    </row>
+    <row r="36" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A36" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="41">
+        <f>SUM(D36:D38)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="19"/>
+      <c r="G36" s="41">
+        <f>SUM(F36:F38)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="31" t="s">
+        <v>67</v>
+      </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -6362,15 +6545,19 @@
       <c r="S36" s="4"/>
       <c r="T36" s="4"/>
     </row>
-    <row r="37" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
+    <row r="37" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="39"/>
+      <c r="B37" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="31" t="s">
+        <v>67</v>
+      </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -6384,8 +6571,236 @@
       <c r="S37" s="4"/>
       <c r="T37" s="4"/>
     </row>
+    <row r="38" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A38" s="40"/>
+      <c r="B38" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+    </row>
+    <row r="39" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="5"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+    </row>
+    <row r="40" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="5"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+    </row>
+    <row r="41" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A41" s="5"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+    </row>
+    <row r="42" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+    </row>
+    <row r="43" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+    </row>
+    <row r="44" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+    </row>
+    <row r="45" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+    </row>
+    <row r="46" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+    </row>
+    <row r="47" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="A12:A35"/>
+    <mergeCell ref="E12:E35"/>
+    <mergeCell ref="G12:G35"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A11"/>
@@ -6393,19 +6808,6 @@
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="G7:G11"/>
     <mergeCell ref="G4:G6"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="A12:A25"/>
-    <mergeCell ref="E12:E25"/>
-    <mergeCell ref="G12:G25"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:I6">
     <cfRule type="expression" dxfId="127" priority="2">
@@ -6593,35 +6995,35 @@
       </c>
       <c r="B5" s="11">
         <f>SUM('Sprint Backlog'!D:D)</f>
-        <v>20</v>
+        <v>26.5</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>17.5</v>
+        <v>23.1875</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>19.875</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>16.5625</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>13.25</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>9.9375</v>
       </c>
       <c r="H5" s="12">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6.625</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>3.3125</v>
       </c>
       <c r="J5" s="12">
         <f t="shared" si="1"/>
@@ -6629,11 +7031,11 @@
       </c>
       <c r="K5" s="12">
         <f>SUM(C5:J5)</f>
-        <v>70</v>
+        <v>92.75</v>
       </c>
       <c r="L5" s="12">
         <f>K5/A$3</f>
-        <v>8.75</v>
+        <v>11.59375</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -6649,47 +7051,47 @@
       </c>
       <c r="B6" s="11">
         <f>B5</f>
-        <v>20</v>
+        <v>26.5</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>20</v>
+        <v>26.5</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="2"/>
-        <v>12.25</v>
+        <v>18.75</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="2"/>
-        <v>6.25</v>
+        <v>12.75</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="2"/>
-        <v>2.0499999999999998</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="G6" s="12">
         <f t="shared" si="2"/>
-        <v>-4.95</v>
+        <v>1.5500000000000007</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="2"/>
-        <v>-12.7</v>
+        <v>-6.1999999999999993</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="2"/>
-        <v>-18.2</v>
+        <v>-11.7</v>
       </c>
       <c r="J6" s="12">
         <f t="shared" si="2"/>
-        <v>-25.7</v>
+        <v>-19.2</v>
       </c>
       <c r="K6" s="12">
         <f>SUM(C6:J6)</f>
-        <v>-21.000000000000004</v>
+        <v>30.999999999999989</v>
       </c>
       <c r="L6" s="12">
         <f>K6/A$3</f>
-        <v>-2.6250000000000004</v>
+        <v>3.8749999999999987</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -6753,7 +7155,7 @@
       </c>
       <c r="B9" s="15">
         <f>B5/A3</f>
-        <v>2.5</v>
+        <v>3.3125</v>
       </c>
       <c r="C9" s="15">
         <f t="shared" ref="C9:K9" si="3">SUM(C10:C12)</f>
@@ -6907,7 +7309,7 @@
       </c>
       <c r="B12" s="17">
         <f>Izaquiel!B9</f>
-        <v>0.75</v>
+        <v>1.5625</v>
       </c>
       <c r="C12" s="12">
         <f>Izaquiel!C9</f>
@@ -8312,18 +8714,6 @@
     <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
@@ -8340,6 +8730,18 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <conditionalFormatting sqref="N10:O19 N21:O22 L20:M20 C21:L102 A20:J20 C10:L19">
     <cfRule type="expression" dxfId="29" priority="2">
@@ -8536,35 +8938,35 @@
       </c>
       <c r="B5" s="11">
         <f>SUMIF('Sprint Backlog'!C:C,"=Izaquiel",'Sprint Backlog'!D:D)</f>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>5.25</v>
+        <v>10.9375</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>9.375</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>3.75</v>
+        <v>7.8125</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6.25</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="1"/>
-        <v>2.25</v>
+        <v>4.6875</v>
       </c>
       <c r="H5" s="12">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>3.125</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>1.5625</v>
       </c>
       <c r="J5" s="12">
         <f t="shared" si="1"/>
@@ -8572,11 +8974,11 @@
       </c>
       <c r="K5" s="12">
         <f>SUM(C5:J5)</f>
-        <v>21</v>
+        <v>43.75</v>
       </c>
       <c r="L5" s="12">
         <f>K5/A$3</f>
-        <v>2.625</v>
+        <v>5.46875</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -8592,47 +8994,47 @@
       </c>
       <c r="B6" s="11">
         <f>B5</f>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="G6" s="12">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="J6" s="12">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="K6" s="12">
         <f>SUM(C6:J6)</f>
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="L6" s="12">
         <f>K6/A$3</f>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -8696,7 +9098,7 @@
       </c>
       <c r="B9" s="15">
         <f>B5/A3</f>
-        <v>0.75</v>
+        <v>1.5625</v>
       </c>
       <c r="C9" s="15">
         <f>SUM(C10:C32)</f>
@@ -9075,14 +9477,6 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
@@ -9098,6 +9492,14 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:L98 K10:L10 A14:A17">
     <cfRule type="expression" dxfId="24" priority="17">
@@ -9880,14 +10282,6 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C1:L1"/>
@@ -9903,6 +10297,14 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:L96">
     <cfRule type="expression" dxfId="9" priority="19">

</xml_diff>

<commit_message>
Integração de remoção, inserção e busca de usuarios com o banco
</commit_message>
<xml_diff>
--- a/Sprint 8/Sprint_8 Burndown-Backlog.xlsx
+++ b/Sprint 8/Sprint_8 Burndown-Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izaquiel\Desktop\projetoPdsTeste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSI\4-Periodo\PDS\SistemaC\SistemaC\Sprint 8\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="105">
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
@@ -159,9 +159,6 @@
 31/10/2016</t>
   </si>
   <si>
-    <t xml:space="preserve">Estudo da biblioteca </t>
-  </si>
-  <si>
     <t>Mudança de métodos das telas de cadastro para classe funcionário</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
   </si>
   <si>
     <t>Integração com agendamento</t>
-  </si>
-  <si>
-    <t>Criação do banco, tabelas e atributos do banco</t>
   </si>
   <si>
     <t>Implementar parte gráfica da tela consulta de agendamentos</t>
@@ -208,30 +202,6 @@
   </si>
   <si>
     <t>Métodos de salvar prontuário</t>
-  </si>
-  <si>
-    <t>Diagrama Entidade Relacionamento</t>
-  </si>
-  <si>
-    <t>Conexão do banco com o eclipse</t>
-  </si>
-  <si>
-    <t>Métodos de inserção de pacientes</t>
-  </si>
-  <si>
-    <t>Métodos de inserção de funcionarios</t>
-  </si>
-  <si>
-    <t>Métodos de remoção de pacientes</t>
-  </si>
-  <si>
-    <t>Métodos de remoção de funcionarios</t>
-  </si>
-  <si>
-    <t>Métodos de busca de pacientes</t>
-  </si>
-  <si>
-    <t>Métodos de busca de funcionários</t>
   </si>
   <si>
     <t>Implementação gráfica da tela de login</t>
@@ -375,6 +345,21 @@
   <si>
     <t>Teste de inserção e consulta de paciente</t>
   </si>
+  <si>
+    <t>Tela de Informações do paciente</t>
+  </si>
+  <si>
+    <t>Implementação gráfica</t>
+  </si>
+  <si>
+    <t>Implementação de métodos e atributos</t>
+  </si>
+  <si>
+    <t>Integração com o sistema</t>
+  </si>
+  <si>
+    <t>Atualizar diagrama de entidade relacionamento</t>
+  </si>
 </sst>
 </file>
 
@@ -384,7 +369,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="[$R$ -416]#,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -488,8 +473,15 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,6 +540,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor rgb="FF003366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1155CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1155CC"/>
+        <bgColor rgb="FFB7B7B7"/>
       </patternFill>
     </fill>
   </fills>
@@ -653,17 +657,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -677,11 +670,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -761,10 +765,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -774,18 +775,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -802,6 +791,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -840,7 +841,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -849,11 +850,35 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="128">
+  <dxfs count="131">
     <dxf>
       <fill>
         <patternFill>
@@ -2610,6 +2635,48 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF1C4587"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF1C4587"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -2701,6 +2768,11 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF1155CC"/>
+      <color rgb="FF0066FF"/>
+      <color rgb="FF0000FF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2833,28 +2905,28 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>26.5</c:v>
+                  <c:v>37.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.1875</c:v>
+                  <c:v>32.59375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.875</c:v>
+                  <c:v>27.9375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.5625</c:v>
+                  <c:v>23.28125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.25</c:v>
+                  <c:v>18.625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.9375</c:v>
+                  <c:v>13.96875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.625</c:v>
+                  <c:v>9.3125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3125</c:v>
+                  <c:v>4.65625</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2966,31 +3038,31 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>26.5</c:v>
+                  <c:v>37.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.5</c:v>
+                  <c:v>36.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>33.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>18.75</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>12.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.5500000000000007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5500000000000007</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-6.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-11.7</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>-19.2</c:v>
+                  <c:v>18.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3018,11 +3090,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="171664408"/>
-        <c:axId val="171665976"/>
+        <c:axId val="208896808"/>
+        <c:axId val="208963272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="171664408"/>
+        <c:axId val="208896808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3103,7 +3175,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="171665976"/>
+        <c:crossAx val="208963272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3111,7 +3183,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171665976"/>
+        <c:axId val="208963272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3162,6 +3234,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -3193,7 +3266,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="171664408"/>
+        <c:crossAx val="208896808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3206,6 +3279,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3241,7 +3315,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.0783405061112067E-2"/>
+          <c:y val="2.8137239602899839E-2"/>
+          <c:w val="0.83849530039593734"/>
+          <c:h val="0.67196043640174696"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="1"/>
@@ -3342,28 +3426,28 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>14</c:v>
+                  <c:v>23.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.25</c:v>
+                  <c:v>20.78125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.5</c:v>
+                  <c:v>17.8125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.75</c:v>
+                  <c:v>14.84375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>11.875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.25</c:v>
+                  <c:v>8.90625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v>5.9375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.75</c:v>
+                  <c:v>2.96875</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3475,31 +3559,31 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>14</c:v>
+                  <c:v>23.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>20.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>12.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>11.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3527,11 +3611,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="171666760"/>
-        <c:axId val="171663232"/>
+        <c:axId val="208516728"/>
+        <c:axId val="209132824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="171666760"/>
+        <c:axId val="208516728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3573,6 +3657,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3604,7 +3689,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="171663232"/>
+        <c:crossAx val="209132824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3612,7 +3697,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171663232"/>
+        <c:axId val="209132824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3663,6 +3748,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -3694,7 +3780,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="171666760"/>
+        <c:crossAx val="208516728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3707,6 +3793,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4028,11 +4115,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="173612960"/>
-        <c:axId val="173613352"/>
+        <c:axId val="209985816"/>
+        <c:axId val="209118944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173612960"/>
+        <c:axId val="209985816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4074,6 +4161,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4105,7 +4193,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173613352"/>
+        <c:crossAx val="209118944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4113,7 +4201,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173613352"/>
+        <c:axId val="209118944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4164,6 +4252,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4195,7 +4284,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173612960"/>
+        <c:crossAx val="209985816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4208,6 +4297,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4344,28 +4434,28 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4477,31 +4567,31 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4529,11 +4619,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="173610608"/>
-        <c:axId val="173609824"/>
+        <c:axId val="209478304"/>
+        <c:axId val="209685024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173610608"/>
+        <c:axId val="209478304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4575,6 +4665,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4606,7 +4697,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173609824"/>
+        <c:crossAx val="209685024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4614,7 +4705,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173609824"/>
+        <c:axId val="209685024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4665,6 +4756,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4696,7 +4788,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173610608"/>
+        <c:crossAx val="209478304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4709,6 +4801,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4775,15 +4868,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47340</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>309600</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>80430</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>300075</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>109005</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5175,10 +5268,10 @@
   <sheetPr>
     <tabColor rgb="FF38761D"/>
   </sheetPr>
-  <dimension ref="A1:AB47"/>
+  <dimension ref="A1:AB51"/>
   <sheetViews>
-    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5195,16 +5288,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
       <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5229,27 +5322,27 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34" t="s">
+      <c r="E2" s="39"/>
+      <c r="F2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34" t="s">
+      <c r="G2" s="39"/>
+      <c r="H2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="34">
+      <c r="I2" s="39">
         <v>8</v>
       </c>
       <c r="J2" s="3"/>
@@ -5273,9 +5366,9 @@
       <c r="AB2" s="4"/>
     </row>
     <row r="3" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -5288,8 +5381,8 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -5311,11 +5404,11 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
-        <v>70</v>
+      <c r="A4" s="40" t="s">
+        <v>60</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>22</v>
@@ -5323,22 +5416,22 @@
       <c r="D4" s="24">
         <v>1</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="36">
         <f>SUM(D4:D6)</f>
         <v>4</v>
       </c>
       <c r="F4" s="24">
         <v>1</v>
       </c>
-      <c r="G4" s="41">
+      <c r="G4" s="36">
         <f>SUM(F4:F6)</f>
         <v>3.5</v>
       </c>
-      <c r="H4" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="30"/>
+      <c r="H4" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="65"/>
+      <c r="J4" s="29"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -5359,9 +5452,9 @@
       <c r="AB4" s="4"/>
     </row>
     <row r="5" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="20" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>22</v>
@@ -5369,15 +5462,15 @@
       <c r="D5" s="24">
         <v>1</v>
       </c>
-      <c r="E5" s="42"/>
+      <c r="E5" s="37"/>
       <c r="F5" s="24">
         <v>1</v>
       </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="I5" s="29"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="28"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -5399,9 +5492,9 @@
       <c r="AB5" s="4"/>
     </row>
     <row r="6" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="21" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>22</v>
@@ -5409,15 +5502,15 @@
       <c r="D6" s="26">
         <v>2</v>
       </c>
-      <c r="E6" s="43"/>
+      <c r="E6" s="38"/>
       <c r="F6" s="26">
         <v>1.5</v>
       </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="I6" s="29"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="28"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -5439,11 +5532,11 @@
       <c r="AB6" s="4"/>
     </row>
     <row r="7" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
-        <v>73</v>
+      <c r="A7" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>22</v>
@@ -5451,19 +5544,19 @@
       <c r="D7" s="27">
         <v>2</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="36">
         <f>SUM(D7:D11)</f>
         <v>10</v>
       </c>
       <c r="F7" s="27">
         <v>2</v>
       </c>
-      <c r="G7" s="41">
+      <c r="G7" s="36">
         <f>SUM(F7:F11)</f>
         <v>8.5</v>
       </c>
-      <c r="H7" s="31" t="s">
-        <v>95</v>
+      <c r="H7" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -5485,9 +5578,9 @@
       <c r="AB7" s="4"/>
     </row>
     <row r="8" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="21" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>22</v>
@@ -5495,13 +5588,13 @@
       <c r="D8" s="19">
         <v>2</v>
       </c>
-      <c r="E8" s="42"/>
+      <c r="E8" s="37"/>
       <c r="F8" s="19">
         <v>1.5</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="31" t="s">
-        <v>95</v>
+      <c r="G8" s="37"/>
+      <c r="H8" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -5523,9 +5616,9 @@
       <c r="AB8" s="4"/>
     </row>
     <row r="9" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="39"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="22" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>22</v>
@@ -5533,13 +5626,13 @@
       <c r="D9" s="19">
         <v>1</v>
       </c>
-      <c r="E9" s="42"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="19">
         <v>1</v>
       </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="31" t="s">
-        <v>95</v>
+      <c r="G9" s="37"/>
+      <c r="H9" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I9" s="5"/>
       <c r="K9" s="4"/>
@@ -5562,9 +5655,9 @@
       <c r="AB9" s="4"/>
     </row>
     <row r="10" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="39"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="23" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>22</v>
@@ -5572,13 +5665,13 @@
       <c r="D10" s="19">
         <v>3</v>
       </c>
-      <c r="E10" s="42"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="19">
         <v>2.5</v>
       </c>
-      <c r="G10" s="42"/>
-      <c r="H10" s="31" t="s">
-        <v>95</v>
+      <c r="G10" s="37"/>
+      <c r="H10" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I10" s="5"/>
       <c r="K10" s="4"/>
@@ -5601,9 +5694,9 @@
       <c r="AB10" s="4"/>
     </row>
     <row r="11" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="22" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>22</v>
@@ -5611,13 +5704,13 @@
       <c r="D11" s="19">
         <v>2</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="19">
         <v>1.5</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="31" t="s">
-        <v>95</v>
+      <c r="G11" s="38"/>
+      <c r="H11" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I11" s="5"/>
       <c r="K11" s="4"/>
@@ -5640,11 +5733,11 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="33" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>24</v>
@@ -5652,19 +5745,19 @@
       <c r="D12" s="19">
         <v>2</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="36">
         <f>SUM(D12:D35)</f>
-        <v>12.5</v>
+        <v>17.75</v>
       </c>
       <c r="F12" s="19">
         <v>1.25</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="36">
         <f>SUM(F12:F35)</f>
-        <v>9.75</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>95</v>
+        <v>13.25</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I12" s="5"/>
       <c r="K12" s="4"/>
@@ -5687,9 +5780,9 @@
       <c r="AB12" s="4"/>
     </row>
     <row r="13" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="39"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="23" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>24</v>
@@ -5697,13 +5790,13 @@
       <c r="D13" s="19">
         <v>2</v>
       </c>
-      <c r="E13" s="42"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="19">
         <v>1.5</v>
       </c>
-      <c r="G13" s="42"/>
-      <c r="H13" s="31" t="s">
-        <v>95</v>
+      <c r="G13" s="37"/>
+      <c r="H13" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I13" s="5"/>
       <c r="K13" s="4"/>
@@ -5726,9 +5819,9 @@
       <c r="AB13" s="4"/>
     </row>
     <row r="14" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="39"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="23" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>24</v>
@@ -5736,13 +5829,13 @@
       <c r="D14" s="19">
         <v>1</v>
       </c>
-      <c r="E14" s="42"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="19">
         <v>1</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="31" t="s">
-        <v>95</v>
+      <c r="G14" s="37"/>
+      <c r="H14" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I14" s="5"/>
       <c r="K14" s="4"/>
@@ -5765,9 +5858,9 @@
       <c r="AB14" s="4"/>
     </row>
     <row r="15" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="23" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>24</v>
@@ -5775,13 +5868,13 @@
       <c r="D15" s="19">
         <v>1</v>
       </c>
-      <c r="E15" s="42"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="19">
         <v>1</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="31" t="s">
-        <v>95</v>
+      <c r="G15" s="37"/>
+      <c r="H15" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I15" s="5"/>
       <c r="K15" s="4"/>
@@ -5804,17 +5897,17 @@
       <c r="AB15" s="4"/>
     </row>
     <row r="16" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="39"/>
-      <c r="B16" s="33" t="s">
-        <v>68</v>
+      <c r="A16" s="34"/>
+      <c r="B16" s="32" t="s">
+        <v>58</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="42"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="19"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="31" t="s">
-        <v>67</v>
+      <c r="G16" s="37"/>
+      <c r="H16" s="30" t="s">
+        <v>57</v>
       </c>
       <c r="I16" s="5"/>
       <c r="K16" s="4"/>
@@ -5837,17 +5930,17 @@
       <c r="AB16" s="4"/>
     </row>
     <row r="17" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="39"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="23" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="42"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="31" t="s">
-        <v>67</v>
+      <c r="G17" s="37"/>
+      <c r="H17" s="30" t="s">
+        <v>57</v>
       </c>
       <c r="I17" s="5"/>
       <c r="K17" s="4"/>
@@ -5870,9 +5963,9 @@
       <c r="AB17" s="4"/>
     </row>
     <row r="18" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="23" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>24</v>
@@ -5880,13 +5973,13 @@
       <c r="D18" s="19">
         <v>1</v>
       </c>
-      <c r="E18" s="42"/>
+      <c r="E18" s="37"/>
       <c r="F18" s="19">
         <v>1</v>
       </c>
-      <c r="G18" s="42"/>
-      <c r="H18" s="31" t="s">
-        <v>95</v>
+      <c r="G18" s="37"/>
+      <c r="H18" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I18" s="5"/>
       <c r="K18" s="4"/>
@@ -5909,9 +6002,9 @@
       <c r="AB18" s="4"/>
     </row>
     <row r="19" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="39"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="23" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>24</v>
@@ -5919,13 +6012,13 @@
       <c r="D19" s="19">
         <v>1</v>
       </c>
-      <c r="E19" s="42"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="19">
         <v>1</v>
       </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="31" t="s">
-        <v>95</v>
+      <c r="G19" s="37"/>
+      <c r="H19" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I19" s="5"/>
       <c r="K19" s="4"/>
@@ -5948,9 +6041,9 @@
       <c r="AB19" s="4"/>
     </row>
     <row r="20" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="39"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="23" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>24</v>
@@ -5958,13 +6051,13 @@
       <c r="D20" s="19">
         <v>1</v>
       </c>
-      <c r="E20" s="42"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="19">
         <v>1</v>
       </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="31" t="s">
-        <v>95</v>
+      <c r="G20" s="37"/>
+      <c r="H20" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I20" s="5"/>
       <c r="K20" s="4"/>
@@ -5987,9 +6080,9 @@
       <c r="AB20" s="4"/>
     </row>
     <row r="21" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="39"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="23" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>24</v>
@@ -5997,13 +6090,13 @@
       <c r="D21" s="19">
         <v>0.25</v>
       </c>
-      <c r="E21" s="42"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="19">
         <v>0.25</v>
       </c>
-      <c r="G21" s="42"/>
-      <c r="H21" s="31" t="s">
-        <v>95</v>
+      <c r="G21" s="37"/>
+      <c r="H21" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I21" s="5"/>
       <c r="K21" s="4"/>
@@ -6026,9 +6119,9 @@
       <c r="AB21" s="4"/>
     </row>
     <row r="22" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="39"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="23" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>24</v>
@@ -6036,13 +6129,13 @@
       <c r="D22" s="19">
         <v>1</v>
       </c>
-      <c r="E22" s="42"/>
+      <c r="E22" s="37"/>
       <c r="F22" s="19">
         <v>0.5</v>
       </c>
-      <c r="G22" s="42"/>
-      <c r="H22" s="31" t="s">
-        <v>95</v>
+      <c r="G22" s="37"/>
+      <c r="H22" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I22" s="5"/>
       <c r="K22" s="4"/>
@@ -6065,9 +6158,9 @@
       <c r="AB22" s="4"/>
     </row>
     <row r="23" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="39"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="23" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>24</v>
@@ -6075,13 +6168,13 @@
       <c r="D23" s="19">
         <v>1</v>
       </c>
-      <c r="E23" s="42"/>
+      <c r="E23" s="37"/>
       <c r="F23" s="19">
         <v>0.5</v>
       </c>
-      <c r="G23" s="42"/>
-      <c r="H23" s="31" t="s">
-        <v>95</v>
+      <c r="G23" s="37"/>
+      <c r="H23" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I23" s="5"/>
       <c r="K23" s="4"/>
@@ -6104,9 +6197,9 @@
       <c r="AB23" s="4"/>
     </row>
     <row r="24" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="39"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="23" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>24</v>
@@ -6114,13 +6207,13 @@
       <c r="D24" s="19">
         <v>1</v>
       </c>
-      <c r="E24" s="42"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="19">
         <v>0.5</v>
       </c>
-      <c r="G24" s="42"/>
-      <c r="H24" s="31" t="s">
-        <v>95</v>
+      <c r="G24" s="37"/>
+      <c r="H24" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I24" s="5"/>
       <c r="K24" s="4"/>
@@ -6143,9 +6236,9 @@
       <c r="AB24" s="4"/>
     </row>
     <row r="25" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="39"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="23" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>24</v>
@@ -6153,13 +6246,13 @@
       <c r="D25" s="19">
         <v>0.25</v>
       </c>
-      <c r="E25" s="42"/>
+      <c r="E25" s="37"/>
       <c r="F25" s="19">
         <v>0.25</v>
       </c>
-      <c r="G25" s="42"/>
-      <c r="H25" s="31" t="s">
-        <v>95</v>
+      <c r="G25" s="37"/>
+      <c r="H25" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I25" s="5"/>
       <c r="K25" s="4"/>
@@ -6182,17 +6275,23 @@
       <c r="AB25" s="4"/>
     </row>
     <row r="26" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="39"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="31" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="E26" s="37"/>
+      <c r="F26" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="37"/>
+      <c r="H26" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I26" s="5"/>
       <c r="K26" s="4"/>
@@ -6215,17 +6314,23 @@
       <c r="AB26" s="4"/>
     </row>
     <row r="27" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="39"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="E27" s="37"/>
+      <c r="F27" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="37"/>
+      <c r="H27" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I27" s="5"/>
       <c r="K27" s="4"/>
@@ -6248,17 +6353,23 @@
       <c r="AB27" s="4"/>
     </row>
     <row r="28" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="39"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="E28" s="37"/>
+      <c r="F28" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="37"/>
+      <c r="H28" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I28" s="5"/>
       <c r="K28" s="4"/>
@@ -6281,17 +6392,23 @@
       <c r="AB28" s="4"/>
     </row>
     <row r="29" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="39"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="31" t="s">
         <v>67</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="E29" s="37"/>
+      <c r="F29" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="37"/>
+      <c r="H29" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I29" s="5"/>
       <c r="K29" s="4"/>
@@ -6314,17 +6431,23 @@
       <c r="AB29" s="4"/>
     </row>
     <row r="30" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="39"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="31" t="s">
-        <v>67</v>
+        <v>90</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="E30" s="37"/>
+      <c r="F30" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="37"/>
+      <c r="H30" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I30" s="5"/>
       <c r="K30" s="4"/>
@@ -6347,17 +6470,23 @@
       <c r="AB30" s="4"/>
     </row>
     <row r="31" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="39"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="31" t="s">
-        <v>67</v>
+        <v>91</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="E31" s="37"/>
+      <c r="F31" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="37"/>
+      <c r="H31" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I31" s="5"/>
       <c r="K31" s="4"/>
@@ -6380,17 +6509,23 @@
       <c r="AB31" s="4"/>
     </row>
     <row r="32" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="39"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="31" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="E32" s="37"/>
+      <c r="F32" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="37"/>
+      <c r="H32" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="I32" s="5"/>
       <c r="K32" s="4"/>
@@ -6413,17 +6548,17 @@
       <c r="AB32" s="4"/>
     </row>
     <row r="33" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="39"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="21" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
-      <c r="E33" s="42"/>
+      <c r="E33" s="37"/>
       <c r="F33" s="19"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="31" t="s">
-        <v>67</v>
+      <c r="G33" s="37"/>
+      <c r="H33" s="30" t="s">
+        <v>57</v>
       </c>
       <c r="I33" s="5"/>
       <c r="K33" s="4"/>
@@ -6446,17 +6581,17 @@
       <c r="AB33" s="4"/>
     </row>
     <row r="34" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="39"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="21" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
-      <c r="E34" s="42"/>
+      <c r="E34" s="37"/>
       <c r="F34" s="19"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="31" t="s">
-        <v>67</v>
+      <c r="G34" s="37"/>
+      <c r="H34" s="30" t="s">
+        <v>57</v>
       </c>
       <c r="I34" s="5"/>
       <c r="K34" s="4"/>
@@ -6479,17 +6614,17 @@
       <c r="AB34" s="4"/>
     </row>
     <row r="35" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="40"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="21" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
-      <c r="E35" s="43"/>
+      <c r="E35" s="38"/>
       <c r="F35" s="19"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="31" t="s">
-        <v>67</v>
+      <c r="G35" s="38"/>
+      <c r="H35" s="30" t="s">
+        <v>57</v>
       </c>
       <c r="I35" s="5"/>
       <c r="K35" s="4"/>
@@ -6512,28 +6647,33 @@
       <c r="AB35" s="4"/>
     </row>
     <row r="36" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="41">
+      <c r="A36" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="E36" s="36">
         <f>SUM(D36:D38)</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="19"/>
-      <c r="G36" s="41">
+        <v>4.5</v>
+      </c>
+      <c r="F36" s="19">
+        <v>2</v>
+      </c>
+      <c r="G36" s="36">
         <f>SUM(F36:F38)</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I36" s="5"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
@@ -6544,22 +6684,35 @@
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
       <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
+      <c r="AA36" s="4"/>
+      <c r="AB36" s="4"/>
     </row>
     <row r="37" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="39"/>
-      <c r="B37" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="19">
+        <v>2</v>
+      </c>
+      <c r="E37" s="37"/>
+      <c r="F37" s="19">
+        <v>2</v>
+      </c>
+      <c r="G37" s="37"/>
+      <c r="H37" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I37" s="5"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -6570,22 +6723,35 @@
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
       <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4"/>
+      <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
     </row>
     <row r="38" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="40"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+        <v>103</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="19">
+        <v>1</v>
+      </c>
+      <c r="E38" s="38"/>
+      <c r="F38" s="19">
+        <v>1</v>
+      </c>
+      <c r="G38" s="38"/>
+      <c r="H38" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I38" s="5"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
@@ -6596,15 +6762,36 @@
       <c r="R38" s="4"/>
       <c r="S38" s="4"/>
       <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
+      <c r="Z38" s="4"/>
+      <c r="AA38" s="4"/>
+      <c r="AB38" s="4"/>
     </row>
     <row r="39" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
+      <c r="A39" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="36">
+        <f>SUM(D39:D42)</f>
+        <v>1</v>
+      </c>
+      <c r="F39" s="19"/>
+      <c r="G39" s="36">
+        <f>SUM(F39:F42)</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -6618,14 +6805,19 @@
       <c r="S39" s="4"/>
       <c r="T39" s="4"/>
     </row>
-    <row r="40" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
+    <row r="40" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="34"/>
+      <c r="B40" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -6640,13 +6832,18 @@
       <c r="T40" s="4"/>
     </row>
     <row r="41" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -6661,12 +6858,24 @@
       <c r="T41" s="4"/>
     </row>
     <row r="42" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="19">
+        <v>1</v>
+      </c>
+      <c r="E42" s="38"/>
+      <c r="F42" s="19">
+        <v>1</v>
+      </c>
+      <c r="G42" s="38"/>
+      <c r="H42" s="30" t="s">
+        <v>85</v>
+      </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -6681,6 +6890,7 @@
       <c r="T42" s="4"/>
     </row>
     <row r="43" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A43" s="5"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -6700,7 +6910,8 @@
       <c r="S43" s="4"/>
       <c r="T43" s="4"/>
     </row>
-    <row r="44" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="5"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -6721,8 +6932,7 @@
       <c r="T44" s="4"/>
     </row>
     <row r="45" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+      <c r="A45" s="5"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -6743,8 +6953,6 @@
       <c r="T45" s="4"/>
     </row>
     <row r="46" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -6765,8 +6973,6 @@
       <c r="T46" s="4"/>
     </row>
     <row r="47" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -6786,11 +6992,104 @@
       <c r="S47" s="4"/>
       <c r="T47" s="4"/>
     </row>
+    <row r="48" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+    </row>
+    <row r="49" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+    </row>
+    <row r="50" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+    </row>
+    <row r="51" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="G36:G38"/>
+  <mergeCells count="23">
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="G39:G42"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -6801,13 +7100,9 @@
     <mergeCell ref="A12:A35"/>
     <mergeCell ref="E12:E35"/>
     <mergeCell ref="G12:G35"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="G36:G38"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:I6">
     <cfRule type="expression" dxfId="127" priority="2">
@@ -6831,7 +7126,7 @@
   <sheetViews>
     <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:J4"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6852,20 +7147,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -6924,40 +7219,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="45">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="K3" s="47" t="s">
+      <c r="D3" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="46" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -6969,18 +7264,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -6995,35 +7290,35 @@
       </c>
       <c r="B5" s="11">
         <f>SUM('Sprint Backlog'!D:D)</f>
-        <v>26.5</v>
+        <v>37.25</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>23.1875</v>
+        <v>32.59375</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="1"/>
-        <v>19.875</v>
+        <v>27.9375</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>16.5625</v>
+        <v>23.28125</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="1"/>
-        <v>13.25</v>
+        <v>18.625</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="1"/>
-        <v>9.9375</v>
+        <v>13.96875</v>
       </c>
       <c r="H5" s="12">
         <f t="shared" si="1"/>
-        <v>6.625</v>
+        <v>9.3125</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" si="1"/>
-        <v>3.3125</v>
+        <v>4.65625</v>
       </c>
       <c r="J5" s="12">
         <f t="shared" si="1"/>
@@ -7031,11 +7326,11 @@
       </c>
       <c r="K5" s="12">
         <f>SUM(C5:J5)</f>
-        <v>92.75</v>
+        <v>130.375</v>
       </c>
       <c r="L5" s="12">
         <f>K5/A$3</f>
-        <v>11.59375</v>
+        <v>16.296875</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -7051,47 +7346,47 @@
       </c>
       <c r="B6" s="11">
         <f>B5</f>
-        <v>26.5</v>
+        <v>37.25</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>26.5</v>
+        <v>36.25</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="2"/>
-        <v>18.75</v>
+        <v>33.75</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="2"/>
-        <v>12.75</v>
+        <v>28.75</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="2"/>
-        <v>8.5500000000000007</v>
+        <v>26.25</v>
       </c>
       <c r="G6" s="12">
         <f t="shared" si="2"/>
-        <v>1.5500000000000007</v>
+        <v>24.75</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="2"/>
-        <v>-6.1999999999999993</v>
+        <v>21.75</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="2"/>
-        <v>-11.7</v>
+        <v>18.75</v>
       </c>
       <c r="J6" s="12">
         <f t="shared" si="2"/>
-        <v>-19.2</v>
+        <v>18.75</v>
       </c>
       <c r="K6" s="12">
         <f>SUM(C6:J6)</f>
-        <v>30.999999999999989</v>
+        <v>209</v>
       </c>
       <c r="L6" s="12">
         <f>K6/A$3</f>
-        <v>3.8749999999999987</v>
+        <v>26.125</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -7129,18 +7424,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -7155,47 +7450,47 @@
       </c>
       <c r="B9" s="15">
         <f>B5/A3</f>
-        <v>3.3125</v>
+        <v>4.65625</v>
       </c>
       <c r="C9" s="15">
         <f t="shared" ref="C9:K9" si="3">SUM(C10:C12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="15">
         <f t="shared" si="3"/>
-        <v>7.75</v>
+        <v>2.5</v>
       </c>
       <c r="E9" s="15">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" s="15">
         <f t="shared" si="3"/>
-        <v>4.2</v>
+        <v>2.5</v>
       </c>
       <c r="G9" s="15">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>1.5</v>
       </c>
       <c r="H9" s="15">
         <f t="shared" si="3"/>
-        <v>7.75</v>
+        <v>3</v>
       </c>
       <c r="I9" s="15">
         <f t="shared" si="3"/>
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="J9" s="15">
         <f t="shared" si="3"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="K9" s="15">
         <f t="shared" si="3"/>
-        <v>45.7</v>
+        <v>18.5</v>
       </c>
       <c r="L9" s="15">
         <f>K9/A$3</f>
-        <v>5.7125000000000004</v>
+        <v>2.3125</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
@@ -7211,40 +7506,40 @@
       </c>
       <c r="B10" s="17">
         <f>Diogo!B9</f>
-        <v>1.75</v>
+        <v>2.96875</v>
       </c>
       <c r="C10" s="12">
         <f>Diogo!C9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="12">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="E10" s="12">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="F10" s="12">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="G10" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="H10" s="12">
         <v>3</v>
       </c>
-      <c r="H10" s="12">
-        <v>4.5</v>
-      </c>
       <c r="I10" s="12">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="J10" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="12">
         <f>SUM(C10:J10)</f>
-        <v>16.75</v>
+        <v>18.5</v>
       </c>
       <c r="L10" s="12">
         <f>K10/A$3</f>
-        <v>2.09375</v>
+        <v>2.3125</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
@@ -7260,40 +7555,40 @@
       </c>
       <c r="B11" s="18">
         <f>Ivo!B9</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="C11" s="12">
         <f>Ivo!C9</f>
         <v>0</v>
       </c>
       <c r="D11" s="12">
-        <v>2.25</v>
+        <v>0</v>
       </c>
       <c r="E11" s="12">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="F11" s="12">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G11" s="12">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="H11" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K11" s="12">
         <f>SUM(C11:J11)</f>
-        <v>13.75</v>
+        <v>0</v>
       </c>
       <c r="L11" s="12">
         <f>K11/A$3</f>
-        <v>1.71875</v>
+        <v>0</v>
       </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
@@ -7316,34 +7611,34 @@
         <v>0</v>
       </c>
       <c r="D12" s="12">
-        <v>3.25</v>
+        <v>0</v>
       </c>
       <c r="E12" s="12">
         <f>Izaquiel!E9</f>
         <v>0</v>
       </c>
       <c r="F12" s="12">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="G12" s="12">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="H12" s="12">
-        <v>2.25</v>
+        <v>0</v>
       </c>
       <c r="I12" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J12" s="12">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="K12" s="12">
         <f>SUM(C12:J12)</f>
-        <v>15.2</v>
+        <v>0</v>
       </c>
       <c r="L12" s="12">
         <f>K12/A$3</f>
-        <v>1.9</v>
+        <v>0</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
@@ -7862,17 +8157,17 @@
   <sheetPr>
     <tabColor rgb="FFC9DAF8"/>
   </sheetPr>
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="4" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.7109375"/>
-    <col min="2" max="2" width="11"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="10" width="12.7109375"/>
     <col min="11" max="11" width="8.28515625"/>
     <col min="12" max="12" width="8"/>
@@ -7880,20 +8175,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -7952,40 +8247,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="45">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="K3" s="47" t="s">
+      <c r="D3" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="46" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -7997,18 +8292,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -8023,35 +8318,35 @@
       </c>
       <c r="B5" s="11">
         <f>SUMIF('Sprint Backlog'!C:C,"=Diogo",'Sprint Backlog'!D:D)</f>
-        <v>14</v>
+        <v>23.75</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>12.25</v>
+        <v>20.78125</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>17.8125</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>8.75</v>
+        <v>14.84375</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>11.875</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="1"/>
-        <v>5.25</v>
+        <v>8.90625</v>
       </c>
       <c r="H5" s="12">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>5.9375</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>2.96875</v>
       </c>
       <c r="J5" s="12">
         <f t="shared" si="1"/>
@@ -8059,11 +8354,11 @@
       </c>
       <c r="K5" s="12">
         <f>SUM(C5:J5)</f>
-        <v>49</v>
+        <v>83.125</v>
       </c>
       <c r="L5" s="12">
         <f>K5/A$3</f>
-        <v>6.125</v>
+        <v>10.390625</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -8079,47 +8374,47 @@
       </c>
       <c r="B6" s="11">
         <f>B5</f>
-        <v>14</v>
+        <v>23.75</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>14</v>
+        <v>22.75</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>20.25</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>15.25</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>12.75</v>
       </c>
       <c r="G6" s="12">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>11.25</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>8.25</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>5.25</v>
       </c>
       <c r="J6" s="12">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>5.25</v>
       </c>
       <c r="K6" s="12">
         <f>SUM(C6:J6)</f>
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="L6" s="12">
         <f>K6/A$3</f>
-        <v>14</v>
+        <v>12.625</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -8157,18 +8452,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -8183,35 +8478,35 @@
       </c>
       <c r="B9" s="15">
         <f>B5/A3</f>
-        <v>1.75</v>
+        <v>2.96875</v>
       </c>
       <c r="C9" s="15">
         <f t="shared" ref="C9:L9" si="3">SUM(C10:C12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E9" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(E10:E27)</f>
+        <v>5</v>
       </c>
       <c r="F9" s="15">
         <f>SUM(F10:F19)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="G9" s="15">
-        <f>SUM(G10:G19)</f>
-        <v>0</v>
+        <f>SUM(G10:G27)</f>
+        <v>1.5</v>
       </c>
       <c r="H9" s="15">
-        <f>SUM(H10:H19)</f>
-        <v>0</v>
+        <f>SUM(H10:H27)</f>
+        <v>3</v>
       </c>
       <c r="I9" s="15">
-        <f>SUM(I10:I19)</f>
-        <v>0</v>
+        <f>SUM(I10:I27)</f>
+        <v>3</v>
       </c>
       <c r="J9" s="15">
         <f>SUM(J10:J19)</f>
@@ -8219,11 +8514,11 @@
       </c>
       <c r="K9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="L9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.4375</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
@@ -8234,12 +8529,12 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="54"/>
+      <c r="A10" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="59"/>
       <c r="C10" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="12">
         <v>0</v>
@@ -8264,30 +8559,30 @@
       </c>
       <c r="K10" s="12">
         <f>SUM(C10:J10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="12">
         <f>K10/A$3</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="M10" s="6"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="52"/>
+      <c r="A11" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="59"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
       <c r="D11" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="12">
         <v>0</v>
@@ -8309,30 +8604,30 @@
       </c>
       <c r="K11" s="12">
         <f>SUM(C11:J11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="12">
         <f>K11/A$3</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="M11" s="6"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="52"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="52"/>
+      <c r="A12" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="61"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
       <c r="D12" s="12">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E12" s="12">
         <v>0</v>
@@ -8354,30 +8649,30 @@
       </c>
       <c r="K12" s="12">
         <f>SUM(C12:J12)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L12" s="12">
         <f>K12/A$3</f>
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="M12" s="6"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="52"/>
+      <c r="A13" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="61"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
       <c r="D13" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="12">
         <v>0</v>
@@ -8399,25 +8694,25 @@
       </c>
       <c r="K13" s="12">
         <f t="shared" ref="K13:K19" si="4">SUM(C13:J13)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L13" s="12">
         <f t="shared" ref="L13:L19" si="5">K13/A$3</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="M13" s="6"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="52"/>
+      <c r="A14" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="61"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -8425,7 +8720,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="12">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F14" s="12">
         <v>0</v>
@@ -8444,25 +8739,25 @@
       </c>
       <c r="K14" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L14" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="M14" s="6"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
     </row>
     <row r="15" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="52"/>
+      <c r="A15" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="63"/>
       <c r="C15" s="12">
         <v>0</v>
       </c>
@@ -8470,7 +8765,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="12">
         <v>0</v>
@@ -8489,25 +8784,25 @@
       </c>
       <c r="K15" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="M15" s="6"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="52"/>
+      <c r="A16" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="63"/>
       <c r="C16" s="12">
         <v>0</v>
       </c>
@@ -8515,7 +8810,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="12">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F16" s="12">
         <v>0</v>
@@ -8534,25 +8829,25 @@
       </c>
       <c r="K16" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="L16" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.3125</v>
       </c>
       <c r="M16" s="6"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
     </row>
     <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="52"/>
+      <c r="A17" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="63"/>
       <c r="C17" s="12">
         <v>0</v>
       </c>
@@ -8563,7 +8858,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="12">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G17" s="12">
         <v>0</v>
@@ -8579,25 +8874,25 @@
       </c>
       <c r="K17" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L17" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="M17" s="6"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
     </row>
     <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="52"/>
+      <c r="A18" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="61"/>
       <c r="C18" s="12">
         <v>0</v>
       </c>
@@ -8608,7 +8903,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G18" s="12">
         <v>0</v>
@@ -8624,25 +8919,25 @@
       </c>
       <c r="K18" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L18" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="M18" s="6"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
     </row>
     <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="52"/>
+      <c r="A19" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="61"/>
       <c r="C19" s="12">
         <v>0</v>
       </c>
@@ -8653,7 +8948,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G19" s="12">
         <v>0</v>
@@ -8669,51 +8964,365 @@
       </c>
       <c r="K19" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L19" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="M19" s="6"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
     </row>
     <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K20" s="6"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
+      <c r="A20" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="61"/>
+      <c r="C20" s="12">
+        <v>0</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12">
+        <v>0</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0</v>
+      </c>
+      <c r="J20" s="12">
+        <v>0</v>
+      </c>
+      <c r="K20" s="12">
+        <f t="shared" ref="K20:K24" si="6">SUM(C20:J20)</f>
+        <v>0.5</v>
+      </c>
+      <c r="L20" s="12">
+        <f t="shared" ref="L20:L24" si="7">K20/A$3</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M20" s="31"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
     </row>
     <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="61"/>
+      <c r="C21" s="12">
+        <v>0</v>
+      </c>
+      <c r="D21" s="12">
+        <v>0</v>
+      </c>
+      <c r="E21" s="12">
+        <v>0</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0</v>
+      </c>
+      <c r="G21" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H21" s="12">
+        <v>0</v>
+      </c>
+      <c r="I21" s="12">
+        <v>0</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0</v>
+      </c>
+      <c r="K21" s="12">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="L21" s="12">
+        <f t="shared" si="7"/>
+        <v>6.25E-2</v>
+      </c>
       <c r="M21" s="6"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
     </row>
     <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="61"/>
+      <c r="C22" s="12">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
+        <v>0</v>
+      </c>
+      <c r="J22" s="12">
+        <v>0</v>
+      </c>
+      <c r="K22" s="12">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="L22" s="12">
+        <f t="shared" si="7"/>
+        <v>6.25E-2</v>
+      </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
     </row>
-    <row r="23" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="61"/>
+      <c r="C23" s="12">
+        <v>0</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0</v>
+      </c>
+      <c r="G23" s="12">
+        <v>0</v>
+      </c>
+      <c r="H23" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="12">
+        <v>0</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0</v>
+      </c>
+      <c r="K23" s="12">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="L23" s="12">
+        <f t="shared" si="7"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="61"/>
+      <c r="C24" s="12">
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="12">
+        <v>0</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24" s="12">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="L24" s="12">
+        <f t="shared" si="7"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A25" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="61"/>
+      <c r="C25" s="12">
+        <v>0</v>
+      </c>
+      <c r="D25" s="12">
+        <v>0</v>
+      </c>
+      <c r="E25" s="12">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0</v>
+      </c>
+      <c r="H25" s="12">
+        <v>2</v>
+      </c>
+      <c r="I25" s="12">
+        <v>0</v>
+      </c>
+      <c r="J25" s="12">
+        <v>0</v>
+      </c>
+      <c r="K25" s="12">
+        <f t="shared" ref="K25:K27" si="8">SUM(C25:J25)</f>
+        <v>2</v>
+      </c>
+      <c r="L25" s="12">
+        <f t="shared" ref="L25:L27" si="9">K25/A$3</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="61"/>
+      <c r="C26" s="12">
+        <v>0</v>
+      </c>
+      <c r="D26" s="12">
+        <v>0</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0</v>
+      </c>
+      <c r="I26" s="12">
+        <v>2</v>
+      </c>
+      <c r="J26" s="12">
+        <v>0</v>
+      </c>
+      <c r="K26" s="12">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="L26" s="12">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="61"/>
+      <c r="C27" s="12">
+        <v>0</v>
+      </c>
+      <c r="D27" s="12">
+        <v>0</v>
+      </c>
+      <c r="E27" s="12">
+        <v>0</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0</v>
+      </c>
+      <c r="G27" s="12">
+        <v>0</v>
+      </c>
+      <c r="H27" s="12">
+        <v>0</v>
+      </c>
+      <c r="I27" s="12">
+        <v>1</v>
+      </c>
+      <c r="J27" s="12">
+        <v>0</v>
+      </c>
+      <c r="K27" s="12">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="L27" s="12">
+        <f t="shared" si="9"/>
+        <v>0.125</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="36">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
@@ -8730,40 +9339,28 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
-  <conditionalFormatting sqref="N10:O19 N21:O22 L20:M20 C21:L102 A20:J20 C10:L19">
+  <conditionalFormatting sqref="N10:O19 N21:O22 M20 C10:L102">
     <cfRule type="expression" dxfId="29" priority="2">
-      <formula>LEN(TRIM(A10))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:L102 A20:J20 C10:L19">
+      <formula>LEN(TRIM(C10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:L102">
     <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:L102 A20:J20 C10:L19">
+  <conditionalFormatting sqref="C10:L102">
     <cfRule type="cellIs" dxfId="27" priority="4" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10:B10 A21:B102">
+  <conditionalFormatting sqref="A28:B102">
     <cfRule type="expression" dxfId="26" priority="5">
-      <formula>LEN(TRIM(A10))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10:B10 A21:B102 N10:O19 N21:O22 L20:M20">
+      <formula>LEN(TRIM(A28))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:B102 N10:O19 N21:O22 M20">
     <cfRule type="notContainsText" dxfId="25" priority="6" operator="notContains" text="9875894754())("/>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -8781,7 +9378,7 @@
   <sheetViews>
     <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15:B15"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8795,20 +9392,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -8867,40 +9464,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="45">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="46" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -8912,18 +9509,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -9072,18 +9669,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -9149,10 +9746,10 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="54"/>
+      <c r="A10" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="53"/>
       <c r="C10" s="12">
         <v>0</v>
       </c>
@@ -9194,10 +9791,10 @@
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="54"/>
+      <c r="A11" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="53"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -9239,10 +9836,10 @@
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="58"/>
+      <c r="A12" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="57"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -9284,10 +9881,10 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="58"/>
+      <c r="A13" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="57"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -9322,10 +9919,10 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="56"/>
+      <c r="A14" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="55"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -9360,10 +9957,10 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="56"/>
+      <c r="A15" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="55"/>
       <c r="C15" s="12">
         <v>0</v>
       </c>
@@ -9398,10 +9995,10 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="56"/>
+      <c r="A16" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="55"/>
       <c r="C16" s="12">
         <v>0</v>
       </c>
@@ -9436,10 +10033,10 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="56"/>
+      <c r="A17" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="55"/>
       <c r="C17" s="12">
         <v>0</v>
       </c>
@@ -9477,6 +10074,14 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
@@ -9492,14 +10097,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:L98 K10:L10 A14:A17">
     <cfRule type="expression" dxfId="24" priority="17">
@@ -9584,7 +10181,7 @@
   <dimension ref="A1:S1048576"/>
   <sheetViews>
     <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -9599,20 +10196,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -9671,40 +10268,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="45">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="K3" s="47" t="s">
+      <c r="D3" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="46" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -9716,18 +10313,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -9742,35 +10339,35 @@
       </c>
       <c r="B5" s="11">
         <f>SUMIF('Sprint Backlog'!C:C,"=Ivo",'Sprint Backlog'!D:D)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="H5" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="J5" s="12">
         <f t="shared" si="1"/>
@@ -9778,11 +10375,11 @@
       </c>
       <c r="K5" s="12">
         <f>SUM(C5:J5)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="L5" s="12">
         <f>K5/A$3</f>
-        <v>0</v>
+        <v>0.4375</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -9798,47 +10395,47 @@
       </c>
       <c r="B6" s="11">
         <f>B5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="12">
         <f>SUM(C6:J6)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L6" s="12">
         <f>K6/A$3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -9876,18 +10473,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -9902,7 +10499,7 @@
       </c>
       <c r="B9" s="15">
         <f>B5/A3</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="C9" s="15">
         <f t="shared" ref="C9:L9" si="3">SUM(C10:C30)</f>
@@ -9953,10 +10550,10 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="54"/>
+      <c r="A10" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="53"/>
       <c r="C10" s="12">
         <v>0</v>
       </c>
@@ -9998,10 +10595,10 @@
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="54"/>
+      <c r="A11" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="53"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -10043,10 +10640,10 @@
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="54"/>
+      <c r="A12" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="53"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -10088,10 +10685,10 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="56"/>
+      <c r="A13" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="55"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -10126,10 +10723,10 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="56"/>
+      <c r="A14" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="55"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -10164,10 +10761,10 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="56"/>
+      <c r="A15" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="55"/>
       <c r="C15" s="12">
         <v>0</v>
       </c>
@@ -10202,10 +10799,10 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="56"/>
+      <c r="A16" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="55"/>
       <c r="C16" s="12">
         <v>0</v>
       </c>
@@ -10240,10 +10837,10 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="56"/>
+      <c r="A17" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="55"/>
       <c r="C17" s="12">
         <v>0</v>
       </c>
@@ -10282,6 +10879,14 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C1:L1"/>
@@ -10297,14 +10902,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:L96">
     <cfRule type="expression" dxfId="9" priority="19">

</xml_diff>

<commit_message>
Atualização diagrama de classe
</commit_message>
<xml_diff>
--- a/Sprint 8/Sprint_8 Burndown-Backlog.xlsx
+++ b/Sprint 8/Sprint_8 Burndown-Backlog.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" tabRatio="990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="100">
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
@@ -159,15 +159,6 @@
 31/10/2016</t>
   </si>
   <si>
-    <t>Mudança de métodos das telas de cadastro para classe funcionário</t>
-  </si>
-  <si>
-    <t>Mudança de métodos das telas de busca para classe funcionário</t>
-  </si>
-  <si>
-    <t>Mudanças de métodos das telas de agendamento para classse funcionário</t>
-  </si>
-  <si>
     <t>Implementação gráfica da tela prontuário</t>
   </si>
   <si>
@@ -202,12 +193,6 @@
   </si>
   <si>
     <t>Métodos de salvar prontuário</t>
-  </si>
-  <si>
-    <t>Implementação gráfica da tela de login</t>
-  </si>
-  <si>
-    <t>Implementação de métodos da tela de login</t>
   </si>
   <si>
     <t>Não Feito</t>
@@ -775,6 +760,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -791,18 +791,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -829,25 +817,13 @@
     <xf numFmtId="164" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -856,10 +832,7 @@
     <xf numFmtId="0" fontId="15" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -871,14 +844,26 @@
     <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="131">
+  <dxfs count="128">
     <dxf>
       <fill>
         <patternFill>
@@ -2635,48 +2620,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF1C4587"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF1C4587"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -2905,28 +2848,28 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>37.25</c:v>
+                  <c:v>44.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.59375</c:v>
+                  <c:v>38.71875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.9375</c:v>
+                  <c:v>33.1875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.28125</c:v>
+                  <c:v>27.65625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.625</c:v>
+                  <c:v>22.125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.96875</c:v>
+                  <c:v>16.59375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.3125</c:v>
+                  <c:v>11.0625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.65625</c:v>
+                  <c:v>5.53125</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3038,31 +2981,31 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>37.25</c:v>
+                  <c:v>44.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.25</c:v>
+                  <c:v>43.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>38.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>33.75</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>28.75</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.25</c:v>
+                  <c:v>28.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.75</c:v>
+                  <c:v>26.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.75</c:v>
+                  <c:v>20.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.75</c:v>
+                  <c:v>17.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.75</c:v>
+                  <c:v>16.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3090,11 +3033,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208896808"/>
-        <c:axId val="208963272"/>
+        <c:axId val="165790512"/>
+        <c:axId val="165790904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208896808"/>
+        <c:axId val="165790512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3175,7 +3118,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208963272"/>
+        <c:crossAx val="165790904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3183,7 +3126,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208963272"/>
+        <c:axId val="165790904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3266,7 +3209,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208896808"/>
+        <c:crossAx val="165790512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3611,11 +3554,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208516728"/>
-        <c:axId val="209132824"/>
+        <c:axId val="165791688"/>
+        <c:axId val="165792080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208516728"/>
+        <c:axId val="165791688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3689,7 +3632,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209132824"/>
+        <c:crossAx val="165792080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3697,7 +3640,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209132824"/>
+        <c:axId val="165792080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3780,7 +3723,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208516728"/>
+        <c:crossAx val="165791688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4115,11 +4058,512 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="209985816"/>
-        <c:axId val="209118944"/>
+        <c:axId val="165792864"/>
+        <c:axId val="165793256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209985816"/>
+        <c:axId val="165792864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>DIAS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="222222"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="165793256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="165793256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>TEMPO EM HORAS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47520">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="165792864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Ivo!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25560">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Ivo!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>(hrs)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Terça
+01/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Quarta
+02/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quinta
+03/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sexta
+04/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sábado
+05/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Domingo
+06/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Segunda
+07/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Terça
+08/11/2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Ivo!$B$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1ED5-4BB2-A00B-9F8936EBC51C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Ivo!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25560">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Ivo!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>(hrs)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Terça
+01/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Quarta
+02/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quinta
+03/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sexta
+04/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sábado
+05/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Domingo
+06/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Segunda
+07/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Terça
+08/11/2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Ivo!$B$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1ED5-4BB2-A00B-9F8936EBC51C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="165794040"/>
+        <c:axId val="165794432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="165794040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4193,7 +4637,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209118944"/>
+        <c:crossAx val="165794432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4201,7 +4645,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209118944"/>
+        <c:axId val="165794432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4284,511 +4728,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209985816"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:noFill/>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ivo!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25560">
-              <a:solidFill>
-                <a:srgbClr val="0000FF"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Ivo!$B$3:$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>(hrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Terça
-01/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Quarta
-02/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Quinta
-03/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sexta
-04/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sábado
-05/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Domingo
-06/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Segunda
-07/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Terça
-08/11/2016</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Ivo!$B$5:$J$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.875</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.625</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.375</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.125</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1ED5-4BB2-A00B-9F8936EBC51C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ivo!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25560">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Ivo!$B$3:$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>(hrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Terça
-01/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Quarta
-02/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Quinta
-03/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sexta
-04/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sábado
-05/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Domingo
-06/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Segunda
-07/11/2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Terça
-08/11/2016</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Ivo!$B$6:$J$6</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1ED5-4BB2-A00B-9F8936EBC51C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="209478304"/>
-        <c:axId val="209685024"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="209478304"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>DIAS</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="222222"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="209685024"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="209685024"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>TEMPO EM HORAS</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47520">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="209478304"/>
+        <c:crossAx val="165794040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5270,8 +5210,8 @@
   </sheetPr>
   <dimension ref="A1:AB51"/>
   <sheetViews>
-    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView windowProtection="1" showGridLines="0" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5288,16 +5228,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5322,27 +5262,27 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="39">
+      <c r="I2" s="34">
         <v>8</v>
       </c>
       <c r="J2" s="3"/>
@@ -5366,9 +5306,9 @@
       <c r="AB2" s="4"/>
     </row>
     <row r="3" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -5381,8 +5321,8 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -5404,11 +5344,11 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>60</v>
+      <c r="A4" s="35" t="s">
+        <v>55</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>22</v>
@@ -5416,21 +5356,21 @@
       <c r="D4" s="24">
         <v>1</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="41">
         <f>SUM(D4:D6)</f>
         <v>4</v>
       </c>
       <c r="F4" s="24">
         <v>1</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="41">
         <f>SUM(F4:F6)</f>
         <v>3.5</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" s="65"/>
+        <v>80</v>
+      </c>
+      <c r="I4" s="33"/>
       <c r="J4" s="29"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -5452,9 +5392,9 @@
       <c r="AB4" s="4"/>
     </row>
     <row r="5" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="41"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>22</v>
@@ -5462,13 +5402,13 @@
       <c r="D5" s="24">
         <v>1</v>
       </c>
-      <c r="E5" s="37"/>
+      <c r="E5" s="42"/>
       <c r="F5" s="24">
         <v>1</v>
       </c>
-      <c r="G5" s="37"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I5" s="28"/>
       <c r="J5" s="3"/>
@@ -5492,9 +5432,9 @@
       <c r="AB5" s="4"/>
     </row>
     <row r="6" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>22</v>
@@ -5502,13 +5442,13 @@
       <c r="D6" s="26">
         <v>2</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="43"/>
       <c r="F6" s="26">
         <v>1.5</v>
       </c>
-      <c r="G6" s="38"/>
+      <c r="G6" s="43"/>
       <c r="H6" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="3"/>
@@ -5532,11 +5472,11 @@
       <c r="AB6" s="4"/>
     </row>
     <row r="7" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
-        <v>63</v>
+      <c r="A7" s="38" t="s">
+        <v>58</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>22</v>
@@ -5544,19 +5484,19 @@
       <c r="D7" s="27">
         <v>2</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="41">
         <f>SUM(D7:D11)</f>
         <v>10</v>
       </c>
       <c r="F7" s="27">
         <v>2</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="41">
         <f>SUM(F7:F11)</f>
         <v>8.5</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -5578,9 +5518,9 @@
       <c r="AB7" s="4"/>
     </row>
     <row r="8" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>22</v>
@@ -5588,13 +5528,13 @@
       <c r="D8" s="19">
         <v>2</v>
       </c>
-      <c r="E8" s="37"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="19">
         <v>1.5</v>
       </c>
-      <c r="G8" s="37"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -5616,9 +5556,9 @@
       <c r="AB8" s="4"/>
     </row>
     <row r="9" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="22" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>22</v>
@@ -5626,13 +5566,13 @@
       <c r="D9" s="19">
         <v>1</v>
       </c>
-      <c r="E9" s="37"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="19">
         <v>1</v>
       </c>
-      <c r="G9" s="37"/>
+      <c r="G9" s="42"/>
       <c r="H9" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I9" s="5"/>
       <c r="K9" s="4"/>
@@ -5655,9 +5595,9 @@
       <c r="AB9" s="4"/>
     </row>
     <row r="10" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="23" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>22</v>
@@ -5665,13 +5605,13 @@
       <c r="D10" s="19">
         <v>3</v>
       </c>
-      <c r="E10" s="37"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="19">
         <v>2.5</v>
       </c>
-      <c r="G10" s="37"/>
+      <c r="G10" s="42"/>
       <c r="H10" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I10" s="5"/>
       <c r="K10" s="4"/>
@@ -5694,9 +5634,9 @@
       <c r="AB10" s="4"/>
     </row>
     <row r="11" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="35"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>22</v>
@@ -5704,13 +5644,13 @@
       <c r="D11" s="19">
         <v>2</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="19">
         <v>1.5</v>
       </c>
-      <c r="G11" s="38"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I11" s="5"/>
       <c r="K11" s="4"/>
@@ -5733,11 +5673,11 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="38" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>24</v>
@@ -5745,19 +5685,19 @@
       <c r="D12" s="19">
         <v>2</v>
       </c>
-      <c r="E12" s="36">
+      <c r="E12" s="41">
         <f>SUM(D12:D35)</f>
         <v>17.75</v>
       </c>
       <c r="F12" s="19">
         <v>1.25</v>
       </c>
-      <c r="G12" s="36">
+      <c r="G12" s="41">
         <f>SUM(F12:F35)</f>
         <v>13.25</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I12" s="5"/>
       <c r="K12" s="4"/>
@@ -5780,9 +5720,9 @@
       <c r="AB12" s="4"/>
     </row>
     <row r="13" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="23" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>24</v>
@@ -5790,13 +5730,13 @@
       <c r="D13" s="19">
         <v>2</v>
       </c>
-      <c r="E13" s="37"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="19">
         <v>1.5</v>
       </c>
-      <c r="G13" s="37"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I13" s="5"/>
       <c r="K13" s="4"/>
@@ -5819,9 +5759,9 @@
       <c r="AB13" s="4"/>
     </row>
     <row r="14" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="23" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>24</v>
@@ -5829,13 +5769,13 @@
       <c r="D14" s="19">
         <v>1</v>
       </c>
-      <c r="E14" s="37"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="19">
         <v>1</v>
       </c>
-      <c r="G14" s="37"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I14" s="5"/>
       <c r="K14" s="4"/>
@@ -5858,9 +5798,9 @@
       <c r="AB14" s="4"/>
     </row>
     <row r="15" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="23" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>24</v>
@@ -5868,13 +5808,13 @@
       <c r="D15" s="19">
         <v>1</v>
       </c>
-      <c r="E15" s="37"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="19">
         <v>1</v>
       </c>
-      <c r="G15" s="37"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I15" s="5"/>
       <c r="K15" s="4"/>
@@ -5897,17 +5837,17 @@
       <c r="AB15" s="4"/>
     </row>
     <row r="16" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="32" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="37"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="19"/>
-      <c r="G16" s="37"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="30" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I16" s="5"/>
       <c r="K16" s="4"/>
@@ -5930,17 +5870,17 @@
       <c r="AB16" s="4"/>
     </row>
     <row r="17" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="37"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="37"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="30" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I17" s="5"/>
       <c r="K17" s="4"/>
@@ -5963,9 +5903,9 @@
       <c r="AB17" s="4"/>
     </row>
     <row r="18" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="23" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>24</v>
@@ -5973,13 +5913,13 @@
       <c r="D18" s="19">
         <v>1</v>
       </c>
-      <c r="E18" s="37"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="19">
         <v>1</v>
       </c>
-      <c r="G18" s="37"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I18" s="5"/>
       <c r="K18" s="4"/>
@@ -6002,9 +5942,9 @@
       <c r="AB18" s="4"/>
     </row>
     <row r="19" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="23" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>24</v>
@@ -6012,13 +5952,13 @@
       <c r="D19" s="19">
         <v>1</v>
       </c>
-      <c r="E19" s="37"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="19">
         <v>1</v>
       </c>
-      <c r="G19" s="37"/>
+      <c r="G19" s="42"/>
       <c r="H19" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I19" s="5"/>
       <c r="K19" s="4"/>
@@ -6041,9 +5981,9 @@
       <c r="AB19" s="4"/>
     </row>
     <row r="20" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="23" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>24</v>
@@ -6051,13 +5991,13 @@
       <c r="D20" s="19">
         <v>1</v>
       </c>
-      <c r="E20" s="37"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="19">
         <v>1</v>
       </c>
-      <c r="G20" s="37"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I20" s="5"/>
       <c r="K20" s="4"/>
@@ -6080,9 +6020,9 @@
       <c r="AB20" s="4"/>
     </row>
     <row r="21" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>24</v>
@@ -6090,13 +6030,13 @@
       <c r="D21" s="19">
         <v>0.25</v>
       </c>
-      <c r="E21" s="37"/>
+      <c r="E21" s="42"/>
       <c r="F21" s="19">
         <v>0.25</v>
       </c>
-      <c r="G21" s="37"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I21" s="5"/>
       <c r="K21" s="4"/>
@@ -6119,9 +6059,9 @@
       <c r="AB21" s="4"/>
     </row>
     <row r="22" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="23" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>24</v>
@@ -6129,13 +6069,13 @@
       <c r="D22" s="19">
         <v>1</v>
       </c>
-      <c r="E22" s="37"/>
+      <c r="E22" s="42"/>
       <c r="F22" s="19">
         <v>0.5</v>
       </c>
-      <c r="G22" s="37"/>
+      <c r="G22" s="42"/>
       <c r="H22" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I22" s="5"/>
       <c r="K22" s="4"/>
@@ -6158,9 +6098,9 @@
       <c r="AB22" s="4"/>
     </row>
     <row r="23" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>24</v>
@@ -6168,13 +6108,13 @@
       <c r="D23" s="19">
         <v>1</v>
       </c>
-      <c r="E23" s="37"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="19">
         <v>0.5</v>
       </c>
-      <c r="G23" s="37"/>
+      <c r="G23" s="42"/>
       <c r="H23" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I23" s="5"/>
       <c r="K23" s="4"/>
@@ -6197,9 +6137,9 @@
       <c r="AB23" s="4"/>
     </row>
     <row r="24" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="23" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>24</v>
@@ -6207,13 +6147,13 @@
       <c r="D24" s="19">
         <v>1</v>
       </c>
-      <c r="E24" s="37"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="19">
         <v>0.5</v>
       </c>
-      <c r="G24" s="37"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I24" s="5"/>
       <c r="K24" s="4"/>
@@ -6236,9 +6176,9 @@
       <c r="AB24" s="4"/>
     </row>
     <row r="25" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>24</v>
@@ -6246,13 +6186,13 @@
       <c r="D25" s="19">
         <v>0.25</v>
       </c>
-      <c r="E25" s="37"/>
+      <c r="E25" s="42"/>
       <c r="F25" s="19">
         <v>0.25</v>
       </c>
-      <c r="G25" s="37"/>
+      <c r="G25" s="42"/>
       <c r="H25" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I25" s="5"/>
       <c r="K25" s="4"/>
@@ -6275,9 +6215,9 @@
       <c r="AB25" s="4"/>
     </row>
     <row r="26" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="34"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="21" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>22</v>
@@ -6285,13 +6225,13 @@
       <c r="D26" s="19">
         <v>0.75</v>
       </c>
-      <c r="E26" s="37"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="19">
         <v>0.5</v>
       </c>
-      <c r="G26" s="37"/>
+      <c r="G26" s="42"/>
       <c r="H26" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I26" s="5"/>
       <c r="K26" s="4"/>
@@ -6314,9 +6254,9 @@
       <c r="AB26" s="4"/>
     </row>
     <row r="27" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="34"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="21" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>22</v>
@@ -6324,13 +6264,13 @@
       <c r="D27" s="19">
         <v>0.75</v>
       </c>
-      <c r="E27" s="37"/>
+      <c r="E27" s="42"/>
       <c r="F27" s="19">
         <v>0.5</v>
       </c>
-      <c r="G27" s="37"/>
+      <c r="G27" s="42"/>
       <c r="H27" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I27" s="5"/>
       <c r="K27" s="4"/>
@@ -6353,9 +6293,9 @@
       <c r="AB27" s="4"/>
     </row>
     <row r="28" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="21" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C28" s="19" t="s">
         <v>22</v>
@@ -6363,13 +6303,13 @@
       <c r="D28" s="19">
         <v>0.75</v>
       </c>
-      <c r="E28" s="37"/>
+      <c r="E28" s="42"/>
       <c r="F28" s="19">
         <v>0.5</v>
       </c>
-      <c r="G28" s="37"/>
+      <c r="G28" s="42"/>
       <c r="H28" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I28" s="5"/>
       <c r="K28" s="4"/>
@@ -6392,9 +6332,9 @@
       <c r="AB28" s="4"/>
     </row>
     <row r="29" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="34"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="21" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>22</v>
@@ -6402,13 +6342,13 @@
       <c r="D29" s="19">
         <v>0.75</v>
       </c>
-      <c r="E29" s="37"/>
+      <c r="E29" s="42"/>
       <c r="F29" s="19">
         <v>0.5</v>
       </c>
-      <c r="G29" s="37"/>
+      <c r="G29" s="42"/>
       <c r="H29" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I29" s="5"/>
       <c r="K29" s="4"/>
@@ -6431,9 +6371,9 @@
       <c r="AB29" s="4"/>
     </row>
     <row r="30" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="34"/>
+      <c r="A30" s="39"/>
       <c r="B30" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C30" s="19" t="s">
         <v>22</v>
@@ -6441,13 +6381,13 @@
       <c r="D30" s="19">
         <v>0.75</v>
       </c>
-      <c r="E30" s="37"/>
+      <c r="E30" s="42"/>
       <c r="F30" s="19">
         <v>0.5</v>
       </c>
-      <c r="G30" s="37"/>
+      <c r="G30" s="42"/>
       <c r="H30" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I30" s="5"/>
       <c r="K30" s="4"/>
@@ -6470,9 +6410,9 @@
       <c r="AB30" s="4"/>
     </row>
     <row r="31" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
+      <c r="A31" s="39"/>
       <c r="B31" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>22</v>
@@ -6480,13 +6420,13 @@
       <c r="D31" s="19">
         <v>0.75</v>
       </c>
-      <c r="E31" s="37"/>
+      <c r="E31" s="42"/>
       <c r="F31" s="19">
         <v>0.5</v>
       </c>
-      <c r="G31" s="37"/>
+      <c r="G31" s="42"/>
       <c r="H31" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I31" s="5"/>
       <c r="K31" s="4"/>
@@ -6509,9 +6449,9 @@
       <c r="AB31" s="4"/>
     </row>
     <row r="32" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="34"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="21" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C32" s="19" t="s">
         <v>22</v>
@@ -6519,13 +6459,13 @@
       <c r="D32" s="19">
         <v>0.75</v>
       </c>
-      <c r="E32" s="37"/>
+      <c r="E32" s="42"/>
       <c r="F32" s="19">
         <v>0.5</v>
       </c>
-      <c r="G32" s="37"/>
+      <c r="G32" s="42"/>
       <c r="H32" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I32" s="5"/>
       <c r="K32" s="4"/>
@@ -6548,17 +6488,17 @@
       <c r="AB32" s="4"/>
     </row>
     <row r="33" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="34"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="21" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
-      <c r="E33" s="37"/>
+      <c r="E33" s="42"/>
       <c r="F33" s="19"/>
-      <c r="G33" s="37"/>
+      <c r="G33" s="42"/>
       <c r="H33" s="30" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I33" s="5"/>
       <c r="K33" s="4"/>
@@ -6581,17 +6521,17 @@
       <c r="AB33" s="4"/>
     </row>
     <row r="34" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="34"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="21" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
-      <c r="E34" s="37"/>
+      <c r="E34" s="42"/>
       <c r="F34" s="19"/>
-      <c r="G34" s="37"/>
+      <c r="G34" s="42"/>
       <c r="H34" s="30" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I34" s="5"/>
       <c r="K34" s="4"/>
@@ -6614,17 +6554,17 @@
       <c r="AB34" s="4"/>
     </row>
     <row r="35" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="35"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
-      <c r="E35" s="38"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="19"/>
-      <c r="G35" s="38"/>
+      <c r="G35" s="43"/>
       <c r="H35" s="30" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I35" s="5"/>
       <c r="K35" s="4"/>
@@ -6647,11 +6587,11 @@
       <c r="AB35" s="4"/>
     </row>
     <row r="36" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="33" t="s">
-        <v>100</v>
+      <c r="A36" s="38" t="s">
+        <v>95</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C36" s="19" t="s">
         <v>22</v>
@@ -6659,19 +6599,19 @@
       <c r="D36" s="19">
         <v>1.5</v>
       </c>
-      <c r="E36" s="36">
+      <c r="E36" s="41">
         <f>SUM(D36:D38)</f>
         <v>4.5</v>
       </c>
       <c r="F36" s="19">
         <v>2</v>
       </c>
-      <c r="G36" s="36">
+      <c r="G36" s="41">
         <f>SUM(F36:F38)</f>
         <v>5</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I36" s="5"/>
       <c r="K36" s="4"/>
@@ -6694,9 +6634,9 @@
       <c r="AB36" s="4"/>
     </row>
     <row r="37" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="34"/>
+      <c r="A37" s="39"/>
       <c r="B37" s="21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C37" s="19" t="s">
         <v>22</v>
@@ -6704,13 +6644,13 @@
       <c r="D37" s="19">
         <v>2</v>
       </c>
-      <c r="E37" s="37"/>
+      <c r="E37" s="42"/>
       <c r="F37" s="19">
         <v>2</v>
       </c>
-      <c r="G37" s="37"/>
+      <c r="G37" s="42"/>
       <c r="H37" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I37" s="5"/>
       <c r="K37" s="4"/>
@@ -6733,9 +6673,9 @@
       <c r="AB37" s="4"/>
     </row>
     <row r="38" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="35"/>
+      <c r="A38" s="40"/>
       <c r="B38" s="21" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C38" s="19" t="s">
         <v>22</v>
@@ -6743,13 +6683,13 @@
       <c r="D38" s="19">
         <v>1</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="43"/>
       <c r="F38" s="19">
         <v>1</v>
       </c>
-      <c r="G38" s="38"/>
+      <c r="G38" s="43"/>
       <c r="H38" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I38" s="5"/>
       <c r="K38" s="4"/>
@@ -6772,25 +6712,31 @@
       <c r="AB38" s="4"/>
     </row>
     <row r="39" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="33" t="s">
-        <v>50</v>
+      <c r="A39" s="38" t="s">
+        <v>47</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="36">
+        <v>48</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="19">
+        <v>2</v>
+      </c>
+      <c r="E39" s="41">
         <f>SUM(D39:D42)</f>
-        <v>1</v>
-      </c>
-      <c r="F39" s="19"/>
-      <c r="G39" s="36">
+        <v>8</v>
+      </c>
+      <c r="F39" s="19">
+        <v>2</v>
+      </c>
+      <c r="G39" s="41">
         <f>SUM(F39:F42)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -6806,17 +6752,23 @@
       <c r="T39" s="4"/>
     </row>
     <row r="40" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="34"/>
+      <c r="A40" s="39"/>
       <c r="B40" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="37"/>
+        <v>49</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="19">
+        <v>2</v>
+      </c>
+      <c r="E40" s="42"/>
+      <c r="F40" s="19">
+        <v>3</v>
+      </c>
+      <c r="G40" s="42"/>
       <c r="H40" s="30" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -6832,17 +6784,23 @@
       <c r="T40" s="4"/>
     </row>
     <row r="41" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="34"/>
+      <c r="A41" s="39"/>
       <c r="B41" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="37"/>
+        <v>50</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="19">
+        <v>3</v>
+      </c>
+      <c r="E41" s="42"/>
+      <c r="F41" s="19">
+        <v>3</v>
+      </c>
+      <c r="G41" s="42"/>
       <c r="H41" s="30" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -6858,9 +6816,9 @@
       <c r="T41" s="4"/>
     </row>
     <row r="42" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="34"/>
+      <c r="A42" s="39"/>
       <c r="B42" s="21" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C42" s="19" t="s">
         <v>23</v>
@@ -6868,13 +6826,13 @@
       <c r="D42" s="19">
         <v>1</v>
       </c>
-      <c r="E42" s="38"/>
+      <c r="E42" s="43"/>
       <c r="F42" s="19">
         <v>1</v>
       </c>
-      <c r="G42" s="38"/>
+      <c r="G42" s="43"/>
       <c r="H42" s="30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -7080,13 +7038,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G4:G6"/>
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="E39:E42"/>
     <mergeCell ref="G39:G42"/>
@@ -7103,6 +7054,13 @@
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="E36:E38"/>
     <mergeCell ref="G36:G38"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G4:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:I6">
     <cfRule type="expression" dxfId="127" priority="2">
@@ -7124,9 +7082,9 @@
   </sheetPr>
   <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7147,20 +7105,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -7219,40 +7177,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45">
+      <c r="A3" s="46">
         <v>8</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="J3" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="H3" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="47" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -7264,18 +7222,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -7290,35 +7248,35 @@
       </c>
       <c r="B5" s="11">
         <f>SUM('Sprint Backlog'!D:D)</f>
-        <v>37.25</v>
+        <v>44.25</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>32.59375</v>
+        <v>38.71875</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="1"/>
-        <v>27.9375</v>
+        <v>33.1875</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>23.28125</v>
+        <v>27.65625</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="1"/>
-        <v>18.625</v>
+        <v>22.125</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="1"/>
-        <v>13.96875</v>
+        <v>16.59375</v>
       </c>
       <c r="H5" s="12">
         <f t="shared" si="1"/>
-        <v>9.3125</v>
+        <v>11.0625</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" si="1"/>
-        <v>4.65625</v>
+        <v>5.53125</v>
       </c>
       <c r="J5" s="12">
         <f t="shared" si="1"/>
@@ -7326,11 +7284,11 @@
       </c>
       <c r="K5" s="12">
         <f>SUM(C5:J5)</f>
-        <v>130.375</v>
+        <v>154.875</v>
       </c>
       <c r="L5" s="12">
         <f>K5/A$3</f>
-        <v>16.296875</v>
+        <v>19.359375</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -7346,47 +7304,47 @@
       </c>
       <c r="B6" s="11">
         <f>B5</f>
-        <v>37.25</v>
+        <v>44.25</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>36.25</v>
+        <v>43.25</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="2"/>
-        <v>33.75</v>
+        <v>38.75</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="2"/>
-        <v>28.75</v>
+        <v>33.75</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="2"/>
-        <v>26.25</v>
+        <v>28.25</v>
       </c>
       <c r="G6" s="12">
         <f t="shared" si="2"/>
-        <v>24.75</v>
+        <v>26.75</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="2"/>
-        <v>21.75</v>
+        <v>20.75</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="2"/>
-        <v>18.75</v>
+        <v>17.75</v>
       </c>
       <c r="J6" s="12">
         <f t="shared" si="2"/>
-        <v>18.75</v>
+        <v>16.75</v>
       </c>
       <c r="K6" s="12">
         <f>SUM(C6:J6)</f>
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="L6" s="12">
         <f>K6/A$3</f>
-        <v>26.125</v>
+        <v>28.25</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -7424,18 +7382,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -7450,7 +7408,7 @@
       </c>
       <c r="B9" s="15">
         <f>B5/A3</f>
-        <v>4.65625</v>
+        <v>5.53125</v>
       </c>
       <c r="C9" s="15">
         <f t="shared" ref="C9:K9" si="3">SUM(C10:C12)</f>
@@ -7458,7 +7416,7 @@
       </c>
       <c r="D9" s="15">
         <f t="shared" si="3"/>
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="E9" s="15">
         <f t="shared" si="3"/>
@@ -7466,7 +7424,7 @@
       </c>
       <c r="F9" s="15">
         <f t="shared" si="3"/>
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="G9" s="15">
         <f t="shared" si="3"/>
@@ -7474,7 +7432,7 @@
       </c>
       <c r="H9" s="15">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I9" s="15">
         <f t="shared" si="3"/>
@@ -7482,15 +7440,15 @@
       </c>
       <c r="J9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="15">
         <f t="shared" si="3"/>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
       <c r="L9" s="15">
         <f>K9/A$3</f>
-        <v>2.3125</v>
+        <v>3.4375</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
@@ -7555,40 +7513,40 @@
       </c>
       <c r="B11" s="18">
         <f>Ivo!B9</f>
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="C11" s="12">
         <f>Ivo!C9</f>
         <v>0</v>
       </c>
       <c r="D11" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" s="12">
         <v>0</v>
       </c>
       <c r="F11" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" s="12">
         <v>0</v>
       </c>
       <c r="H11" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I11" s="12">
         <v>0</v>
       </c>
       <c r="J11" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="12">
         <f>SUM(C11:J11)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L11" s="12">
         <f>K11/A$3</f>
-        <v>0</v>
+        <v>1.125</v>
       </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
@@ -8175,20 +8133,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -8247,40 +8205,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45">
+      <c r="A3" s="46">
         <v>8</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="J3" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="H3" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="47" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -8292,18 +8250,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -8452,18 +8410,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -8529,10 +8487,10 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="59"/>
+      <c r="A10" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="56"/>
       <c r="C10" s="12">
         <v>1</v>
       </c>
@@ -8566,18 +8524,18 @@
         <v>0.125</v>
       </c>
       <c r="M10" s="6"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="59"/>
+      <c r="A11" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="56"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -8611,18 +8569,18 @@
         <v>0.125</v>
       </c>
       <c r="M11" s="6"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="51"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="61"/>
+      <c r="A12" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="53"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -8656,18 +8614,18 @@
         <v>0.1875</v>
       </c>
       <c r="M12" s="6"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="61"/>
+      <c r="A13" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="53"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -8709,10 +8667,10 @@
       <c r="S13" s="6"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="61"/>
+      <c r="A14" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="53"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -8754,10 +8712,10 @@
       <c r="S14" s="6"/>
     </row>
     <row r="15" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="63"/>
+      <c r="A15" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="59"/>
       <c r="C15" s="12">
         <v>0</v>
       </c>
@@ -8799,10 +8757,10 @@
       <c r="S15" s="6"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="64" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="63"/>
+      <c r="A16" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="59"/>
       <c r="C16" s="12">
         <v>0</v>
       </c>
@@ -8844,10 +8802,10 @@
       <c r="S16" s="6"/>
     </row>
     <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="63"/>
+      <c r="A17" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="59"/>
       <c r="C17" s="12">
         <v>0</v>
       </c>
@@ -8889,10 +8847,10 @@
       <c r="S17" s="6"/>
     </row>
     <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="60" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="61"/>
+      <c r="A18" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="53"/>
       <c r="C18" s="12">
         <v>0</v>
       </c>
@@ -8934,10 +8892,10 @@
       <c r="S18" s="6"/>
     </row>
     <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="60" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="61"/>
+      <c r="A19" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="53"/>
       <c r="C19" s="12">
         <v>0</v>
       </c>
@@ -8979,10 +8937,10 @@
       <c r="S19" s="6"/>
     </row>
     <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="61"/>
+      <c r="A20" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="53"/>
       <c r="C20" s="12">
         <v>0</v>
       </c>
@@ -9022,10 +8980,10 @@
       <c r="Q20" s="6"/>
     </row>
     <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="61"/>
+      <c r="A21" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="53"/>
       <c r="C21" s="12">
         <v>0</v>
       </c>
@@ -9067,10 +9025,10 @@
       <c r="S21" s="6"/>
     </row>
     <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" s="61"/>
+      <c r="A22" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="53"/>
       <c r="C22" s="12">
         <v>0</v>
       </c>
@@ -9112,10 +9070,10 @@
       <c r="S22" s="6"/>
     </row>
     <row r="23" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" s="61"/>
+      <c r="A23" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="53"/>
       <c r="C23" s="12">
         <v>0</v>
       </c>
@@ -9150,10 +9108,10 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="61"/>
+      <c r="A24" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="53"/>
       <c r="C24" s="12">
         <v>0</v>
       </c>
@@ -9188,10 +9146,10 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" s="61"/>
+      <c r="A25" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="53"/>
       <c r="C25" s="12">
         <v>0</v>
       </c>
@@ -9226,10 +9184,10 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" s="61"/>
+      <c r="A26" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="53"/>
       <c r="C26" s="12">
         <v>0</v>
       </c>
@@ -9264,10 +9222,10 @@
       </c>
     </row>
     <row r="27" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="B27" s="61"/>
+      <c r="A27" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="53"/>
       <c r="C27" s="12">
         <v>0</v>
       </c>
@@ -9303,26 +9261,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
@@ -9339,6 +9277,26 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <conditionalFormatting sqref="N10:O19 N21:O22 M20 C10:L102">
     <cfRule type="expression" dxfId="29" priority="2">
@@ -9392,20 +9350,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -9464,40 +9422,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45">
+      <c r="A3" s="46">
         <v>8</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="47" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -9509,18 +9467,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -9669,18 +9627,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -9746,10 +9704,10 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="53"/>
+      <c r="A10" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="63"/>
       <c r="C10" s="12">
         <v>0</v>
       </c>
@@ -9791,10 +9749,10 @@
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="53"/>
+      <c r="A11" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="63"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -9836,10 +9794,10 @@
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="57"/>
+      <c r="A12" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="65"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -9881,10 +9839,10 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="57"/>
+      <c r="A13" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="65"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -9919,10 +9877,10 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="55"/>
+      <c r="A14" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="61"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -9957,10 +9915,10 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="55"/>
+      <c r="A15" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="61"/>
       <c r="C15" s="12">
         <v>0</v>
       </c>
@@ -9995,10 +9953,10 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="55"/>
+      <c r="A16" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="61"/>
       <c r="C16" s="12">
         <v>0</v>
       </c>
@@ -10033,10 +9991,10 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="55"/>
+      <c r="A17" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="61"/>
       <c r="C17" s="12">
         <v>0</v>
       </c>
@@ -10074,14 +10032,6 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
@@ -10097,6 +10047,14 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:L98 K10:L10 A14:A17">
     <cfRule type="expression" dxfId="24" priority="17">
@@ -10182,7 +10140,7 @@
   <sheetViews>
     <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10196,20 +10154,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -10268,40 +10226,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45">
+      <c r="A3" s="46">
         <v>8</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="J3" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="H3" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="47" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -10313,18 +10271,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -10339,35 +10297,35 @@
       </c>
       <c r="B5" s="11">
         <f>SUMIF('Sprint Backlog'!C:C,"=Ivo",'Sprint Backlog'!D:D)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>0.875</v>
+        <v>7</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>6</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>0.625</v>
+        <v>5</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="1"/>
-        <v>0.375</v>
+        <v>3</v>
       </c>
       <c r="H5" s="12">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" si="1"/>
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="J5" s="12">
         <f t="shared" si="1"/>
@@ -10375,11 +10333,11 @@
       </c>
       <c r="K5" s="12">
         <f>SUM(C5:J5)</f>
-        <v>3.5</v>
+        <v>28</v>
       </c>
       <c r="L5" s="12">
         <f>K5/A$3</f>
-        <v>0.4375</v>
+        <v>3.5</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -10395,47 +10353,47 @@
       </c>
       <c r="B6" s="11">
         <f>B5</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6" s="12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K6" s="12">
         <f>SUM(C6:J6)</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="L6" s="12">
         <f>K6/A$3</f>
-        <v>1</v>
+        <v>3.125</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -10473,18 +10431,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -10499,7 +10457,7 @@
       </c>
       <c r="B9" s="15">
         <f>B5/A3</f>
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="C9" s="15">
         <f t="shared" ref="C9:L9" si="3">SUM(C10:C30)</f>
@@ -10507,7 +10465,7 @@
       </c>
       <c r="D9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="15">
         <f t="shared" si="3"/>
@@ -10515,7 +10473,7 @@
       </c>
       <c r="F9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G9" s="15">
         <f t="shared" si="3"/>
@@ -10523,7 +10481,7 @@
       </c>
       <c r="H9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I9" s="15">
         <f t="shared" si="3"/>
@@ -10531,15 +10489,15 @@
       </c>
       <c r="J9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.125</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
@@ -10550,15 +10508,15 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="53"/>
+      <c r="A10" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="63"/>
       <c r="C10" s="12">
         <v>0</v>
       </c>
       <c r="D10" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" s="12">
         <v>0</v>
@@ -10580,11 +10538,11 @@
       </c>
       <c r="K10" s="12">
         <f>SUM(C10:J10)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" s="12">
         <f>K10/A$3</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
@@ -10595,10 +10553,10 @@
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="53"/>
+      <c r="A11" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="63"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -10609,7 +10567,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" s="12">
         <v>0</v>
@@ -10625,11 +10583,11 @@
       </c>
       <c r="K11" s="12">
         <f>SUM(C11:J11)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L11" s="12">
         <f>K11/A$3</f>
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
@@ -10640,10 +10598,10 @@
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="53"/>
+      <c r="A12" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="63"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -10660,7 +10618,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I12" s="12">
         <v>0</v>
@@ -10670,11 +10628,11 @@
       </c>
       <c r="K12" s="12">
         <f>SUM(C12:J12)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L12" s="12">
         <f>K12/A$3</f>
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
@@ -10685,10 +10643,10 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="55"/>
+      <c r="A13" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="61"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -10711,166 +10669,15 @@
         <v>0</v>
       </c>
       <c r="J13" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="12">
         <f>SUM(C13:J13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="12">
         <f>K13/A$3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="12">
-        <v>0</v>
-      </c>
-      <c r="D14" s="12">
-        <v>0</v>
-      </c>
-      <c r="E14" s="12">
-        <v>0</v>
-      </c>
-      <c r="F14" s="12">
-        <v>0</v>
-      </c>
-      <c r="G14" s="12">
-        <v>0</v>
-      </c>
-      <c r="H14" s="12">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12">
-        <v>0</v>
-      </c>
-      <c r="J14" s="12">
-        <v>0</v>
-      </c>
-      <c r="K14" s="12">
-        <f t="shared" ref="K14:K16" si="4">SUM(C14:J14)</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="12">
-        <f t="shared" ref="L14:L17" si="5">K14/A$3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="12">
-        <v>0</v>
-      </c>
-      <c r="D15" s="12">
-        <v>0</v>
-      </c>
-      <c r="E15" s="12">
-        <v>0</v>
-      </c>
-      <c r="F15" s="12">
-        <v>0</v>
-      </c>
-      <c r="G15" s="12">
-        <v>0</v>
-      </c>
-      <c r="H15" s="12">
-        <v>0</v>
-      </c>
-      <c r="I15" s="12">
-        <v>0</v>
-      </c>
-      <c r="J15" s="12">
-        <v>0</v>
-      </c>
-      <c r="K15" s="12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="12">
-        <v>0</v>
-      </c>
-      <c r="D16" s="12">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12">
-        <v>0</v>
-      </c>
-      <c r="F16" s="12">
-        <v>0</v>
-      </c>
-      <c r="G16" s="12">
-        <v>0</v>
-      </c>
-      <c r="H16" s="12">
-        <v>0</v>
-      </c>
-      <c r="I16" s="12">
-        <v>0</v>
-      </c>
-      <c r="J16" s="12">
-        <v>0</v>
-      </c>
-      <c r="K16" s="12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="12">
-        <v>0</v>
-      </c>
-      <c r="D17" s="12">
-        <v>0</v>
-      </c>
-      <c r="E17" s="12">
-        <v>0</v>
-      </c>
-      <c r="F17" s="12">
-        <v>0</v>
-      </c>
-      <c r="G17" s="12">
-        <v>0</v>
-      </c>
-      <c r="H17" s="12">
-        <v>0</v>
-      </c>
-      <c r="I17" s="12">
-        <v>0</v>
-      </c>
-      <c r="J17" s="12">
-        <v>0</v>
-      </c>
-      <c r="K17" s="12">
-        <v>0</v>
-      </c>
-      <c r="L17" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10878,15 +10685,7 @@
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
+  <mergeCells count="19">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C1:L1"/>
@@ -10902,6 +10701,10 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:L96">
     <cfRule type="expression" dxfId="9" priority="19">
@@ -10926,27 +10729,27 @@
   <conditionalFormatting sqref="A18:B96">
     <cfRule type="notContainsText" dxfId="5" priority="23" operator="notContains" text="9875894754())("/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:L17">
+  <conditionalFormatting sqref="C10:L13">
     <cfRule type="expression" dxfId="4" priority="1">
       <formula>LEN(TRIM(C10))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:L17">
+  <conditionalFormatting sqref="C10:L13">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:L17">
+  <conditionalFormatting sqref="C10:L13">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:A17 A10:B12">
+  <conditionalFormatting sqref="A13 A10:B12">
     <cfRule type="expression" dxfId="1" priority="4">
       <formula>LEN(TRIM(A10))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C17 A13:A17 A10:B12">
+  <conditionalFormatting sqref="C13 A13 A10:B12">
     <cfRule type="notContainsText" dxfId="0" priority="5" operator="notContains" text="9875894754())("/>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Métodos cad e cons de agenda
</commit_message>
<xml_diff>
--- a/Sprint 8/Sprint_8 Burndown-Backlog.xlsx
+++ b/Sprint 8/Sprint_8 Burndown-Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSI\4-Periodo\PDS\SistemaC\SistemaC\Sprint 8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izaquiel\Desktop\projetoPdsTeste\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" tabRatio="990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="106">
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
@@ -198,12 +198,6 @@
     <t>Não Feito</t>
   </si>
   <si>
-    <t>Inserção de agendamentos</t>
-  </si>
-  <si>
-    <t>Busca de agendamentos</t>
-  </si>
-  <si>
     <t>Reajuste de código</t>
   </si>
   <si>
@@ -344,6 +338,30 @@
   </si>
   <si>
     <t>Atualizar diagrama de entidade relacionamento</t>
+  </si>
+  <si>
+    <t>Criação de método cadastro de agenda</t>
+  </si>
+  <si>
+    <t>Criação de método consulta de agenda</t>
+  </si>
+  <si>
+    <t>Criação de método alteração de agenda</t>
+  </si>
+  <si>
+    <t>Teste de inserção e consulta de agenda</t>
+  </si>
+  <si>
+    <t>Criação de método para criação de prontuário de atendimento</t>
+  </si>
+  <si>
+    <t>Criação de método para consulta de prontuário de atendimento</t>
+  </si>
+  <si>
+    <t>Criação de método para alteração de prontuário de atendimento</t>
+  </si>
+  <si>
+    <t>Teste de inserção de consulta de prontuário</t>
   </si>
 </sst>
 </file>
@@ -670,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -759,29 +777,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,6 +793,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -823,6 +840,15 @@
     <xf numFmtId="0" fontId="15" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -834,15 +860,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2848,28 +2865,28 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>44.25</c:v>
+                  <c:v>47.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.71875</c:v>
+                  <c:v>41.5625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.1875</c:v>
+                  <c:v>35.625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.65625</c:v>
+                  <c:v>29.6875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.125</c:v>
+                  <c:v>23.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.59375</c:v>
+                  <c:v>17.8125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.0625</c:v>
+                  <c:v>11.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.53125</c:v>
+                  <c:v>5.9375</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2981,31 +2998,31 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>44.25</c:v>
+                  <c:v>47.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.25</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.75</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.75</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.25</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.75</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.75</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.75</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.75</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3033,11 +3050,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="165790512"/>
-        <c:axId val="165790904"/>
+        <c:axId val="120555136"/>
+        <c:axId val="120554744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="165790512"/>
+        <c:axId val="120555136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3118,7 +3135,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165790904"/>
+        <c:crossAx val="120554744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3126,7 +3143,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165790904"/>
+        <c:axId val="120554744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3209,7 +3226,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165790512"/>
+        <c:crossAx val="120555136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3554,515 +3571,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="165791688"/>
-        <c:axId val="165792080"/>
+        <c:axId val="120556704"/>
+        <c:axId val="120557096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="165791688"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>DIAS</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="222222"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="165792080"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="165792080"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>TEMPO EM HORAS</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47520">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="165791688"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:noFill/>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Izaquiel!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25560">
-              <a:solidFill>
-                <a:srgbClr val="0000FF"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Izaquiel!$B$3:$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>(hrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Terça
-25/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Quarta
-26/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Quinta
-27/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sexta
-28/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sábado
-29/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Domingo
-30/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Segunda
-31/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Terça
-25/10/2016</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Izaquiel!$B$5:$J$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10.9375</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.375</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.8125</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.6875</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.125</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.5625</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5DC1-45E4-B87A-C4BF8E3DF284}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Izaquiel!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25560">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Izaquiel!$B$3:$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>(hrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Terça
-25/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Quarta
-26/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Quinta
-27/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sexta
-28/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sábado
-29/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Domingo
-30/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Segunda
-31/10/2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Terça
-25/10/2016</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Izaquiel!$B$6:$J$6</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5DC1-45E4-B87A-C4BF8E3DF284}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="165792864"/>
-        <c:axId val="165793256"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="165792864"/>
+        <c:axId val="120556704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4135,7 +3648,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165793256"/>
+        <c:crossAx val="120557096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4143,7 +3656,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165793256"/>
+        <c:axId val="120557096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4225,7 +3738,508 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165792864"/>
+        <c:crossAx val="120556704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Izaquiel!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25560">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Izaquiel!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>(hrs)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Terça
+25/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Quarta
+26/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quinta
+27/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sexta
+28/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sábado
+29/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Domingo
+30/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Segunda
+31/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Terça
+25/10/2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Izaquiel!$B$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.78125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.8125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.84375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.90625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.96875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5DC1-45E4-B87A-C4BF8E3DF284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Izaquiel!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25560">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Izaquiel!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>(hrs)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Terça
+25/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Quarta
+26/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quinta
+27/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sexta
+28/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sábado
+29/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Domingo
+30/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Segunda
+31/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Terça
+25/10/2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Izaquiel!$B$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5DC1-45E4-B87A-C4BF8E3DF284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="170329880"/>
+        <c:axId val="170329096"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="170329880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>DIAS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="222222"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="170329096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="170329096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1000" b="1" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>TEMPO EM HORAS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47520">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="170329880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4559,11 +4573,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="165794040"/>
-        <c:axId val="165794432"/>
+        <c:axId val="170326744"/>
+        <c:axId val="170329488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="165794040"/>
+        <c:axId val="170326744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4605,7 +4619,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4637,7 +4650,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165794432"/>
+        <c:crossAx val="170329488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4645,7 +4658,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165794432"/>
+        <c:axId val="170329488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4696,7 +4709,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4728,7 +4740,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165794040"/>
+        <c:crossAx val="170326744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4741,7 +4753,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5208,10 +5219,10 @@
   <sheetPr>
     <tabColor rgb="FF38761D"/>
   </sheetPr>
-  <dimension ref="A1:AB51"/>
+  <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView windowProtection="1" showGridLines="0" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5228,16 +5239,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
       <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5262,27 +5273,27 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34" t="s">
+      <c r="E2" s="38"/>
+      <c r="F2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34" t="s">
+      <c r="G2" s="38"/>
+      <c r="H2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="34">
+      <c r="I2" s="38">
         <v>8</v>
       </c>
       <c r="J2" s="3"/>
@@ -5306,9 +5317,9 @@
       <c r="AB2" s="4"/>
     </row>
     <row r="3" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -5321,8 +5332,8 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -5344,11 +5355,11 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
-        <v>55</v>
+      <c r="A4" s="40" t="s">
+        <v>53</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>22</v>
@@ -5356,21 +5367,21 @@
       <c r="D4" s="24">
         <v>1</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="35">
         <f>SUM(D4:D6)</f>
         <v>4</v>
       </c>
       <c r="F4" s="24">
         <v>1</v>
       </c>
-      <c r="G4" s="41">
+      <c r="G4" s="35">
         <f>SUM(F4:F6)</f>
         <v>3.5</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="33"/>
+        <v>78</v>
+      </c>
+      <c r="I4" s="32"/>
       <c r="J4" s="29"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -5392,9 +5403,9 @@
       <c r="AB4" s="4"/>
     </row>
     <row r="5" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>22</v>
@@ -5402,13 +5413,13 @@
       <c r="D5" s="24">
         <v>1</v>
       </c>
-      <c r="E5" s="42"/>
+      <c r="E5" s="36"/>
       <c r="F5" s="24">
         <v>1</v>
       </c>
-      <c r="G5" s="42"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I5" s="28"/>
       <c r="J5" s="3"/>
@@ -5432,9 +5443,9 @@
       <c r="AB5" s="4"/>
     </row>
     <row r="6" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>22</v>
@@ -5442,13 +5453,13 @@
       <c r="D6" s="26">
         <v>2</v>
       </c>
-      <c r="E6" s="43"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="26">
         <v>1.5</v>
       </c>
-      <c r="G6" s="43"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="3"/>
@@ -5472,11 +5483,11 @@
       <c r="AB6" s="4"/>
     </row>
     <row r="7" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
-        <v>58</v>
+      <c r="A7" s="33" t="s">
+        <v>56</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>22</v>
@@ -5484,19 +5495,19 @@
       <c r="D7" s="27">
         <v>2</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="35">
         <f>SUM(D7:D11)</f>
         <v>10</v>
       </c>
       <c r="F7" s="27">
         <v>2</v>
       </c>
-      <c r="G7" s="41">
+      <c r="G7" s="35">
         <f>SUM(F7:F11)</f>
         <v>8.5</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -5518,9 +5529,9 @@
       <c r="AB7" s="4"/>
     </row>
     <row r="8" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>22</v>
@@ -5528,13 +5539,13 @@
       <c r="D8" s="19">
         <v>2</v>
       </c>
-      <c r="E8" s="42"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="19">
         <v>1.5</v>
       </c>
-      <c r="G8" s="42"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -5556,9 +5567,9 @@
       <c r="AB8" s="4"/>
     </row>
     <row r="9" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="39"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>22</v>
@@ -5566,13 +5577,13 @@
       <c r="D9" s="19">
         <v>1</v>
       </c>
-      <c r="E9" s="42"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="19">
         <v>1</v>
       </c>
-      <c r="G9" s="42"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I9" s="5"/>
       <c r="K9" s="4"/>
@@ -5595,9 +5606,9 @@
       <c r="AB9" s="4"/>
     </row>
     <row r="10" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="39"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>22</v>
@@ -5605,13 +5616,13 @@
       <c r="D10" s="19">
         <v>3</v>
       </c>
-      <c r="E10" s="42"/>
+      <c r="E10" s="36"/>
       <c r="F10" s="19">
         <v>2.5</v>
       </c>
-      <c r="G10" s="42"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I10" s="5"/>
       <c r="K10" s="4"/>
@@ -5634,9 +5645,9 @@
       <c r="AB10" s="4"/>
     </row>
     <row r="11" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>22</v>
@@ -5644,13 +5655,13 @@
       <c r="D11" s="19">
         <v>2</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="19">
         <v>1.5</v>
       </c>
-      <c r="G11" s="43"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I11" s="5"/>
       <c r="K11" s="4"/>
@@ -5673,11 +5684,11 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="33" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>24</v>
@@ -5685,19 +5696,19 @@
       <c r="D12" s="19">
         <v>2</v>
       </c>
-      <c r="E12" s="41">
-        <f>SUM(D12:D35)</f>
-        <v>17.75</v>
+      <c r="E12" s="35">
+        <f>SUM(D12:D41)</f>
+        <v>21</v>
       </c>
       <c r="F12" s="19">
         <v>1.25</v>
       </c>
-      <c r="G12" s="41">
-        <f>SUM(F12:F35)</f>
-        <v>13.25</v>
+      <c r="G12" s="35">
+        <f>SUM(F12:F41)</f>
+        <v>15.25</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I12" s="5"/>
       <c r="K12" s="4"/>
@@ -5720,9 +5731,9 @@
       <c r="AB12" s="4"/>
     </row>
     <row r="13" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="39"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>24</v>
@@ -5730,13 +5741,13 @@
       <c r="D13" s="19">
         <v>2</v>
       </c>
-      <c r="E13" s="42"/>
+      <c r="E13" s="36"/>
       <c r="F13" s="19">
         <v>1.5</v>
       </c>
-      <c r="G13" s="42"/>
+      <c r="G13" s="36"/>
       <c r="H13" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I13" s="5"/>
       <c r="K13" s="4"/>
@@ -5759,9 +5770,9 @@
       <c r="AB13" s="4"/>
     </row>
     <row r="14" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="39"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>24</v>
@@ -5769,13 +5780,13 @@
       <c r="D14" s="19">
         <v>1</v>
       </c>
-      <c r="E14" s="42"/>
+      <c r="E14" s="36"/>
       <c r="F14" s="19">
         <v>1</v>
       </c>
-      <c r="G14" s="42"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I14" s="5"/>
       <c r="K14" s="4"/>
@@ -5798,9 +5809,9 @@
       <c r="AB14" s="4"/>
     </row>
     <row r="15" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>24</v>
@@ -5808,13 +5819,13 @@
       <c r="D15" s="19">
         <v>1</v>
       </c>
-      <c r="E15" s="42"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="19">
         <v>1</v>
       </c>
-      <c r="G15" s="42"/>
+      <c r="G15" s="36"/>
       <c r="H15" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I15" s="5"/>
       <c r="K15" s="4"/>
@@ -5837,17 +5848,23 @@
       <c r="AB15" s="4"/>
     </row>
     <row r="16" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="39"/>
-      <c r="B16" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="42"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="19">
+        <v>1</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="19">
+        <v>1</v>
+      </c>
+      <c r="G16" s="36"/>
       <c r="H16" s="30" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="I16" s="5"/>
       <c r="K16" s="4"/>
@@ -5870,17 +5887,23 @@
       <c r="AB16" s="4"/>
     </row>
     <row r="17" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="39"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="42"/>
+        <v>86</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="19">
+        <v>1</v>
+      </c>
+      <c r="E17" s="36"/>
+      <c r="F17" s="19">
+        <v>1</v>
+      </c>
+      <c r="G17" s="36"/>
       <c r="H17" s="30" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="I17" s="5"/>
       <c r="K17" s="4"/>
@@ -5903,7 +5926,7 @@
       <c r="AB17" s="4"/>
     </row>
     <row r="18" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="23" t="s">
         <v>87</v>
       </c>
@@ -5913,13 +5936,13 @@
       <c r="D18" s="19">
         <v>1</v>
       </c>
-      <c r="E18" s="42"/>
+      <c r="E18" s="36"/>
       <c r="F18" s="19">
         <v>1</v>
       </c>
-      <c r="G18" s="42"/>
+      <c r="G18" s="36"/>
       <c r="H18" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I18" s="5"/>
       <c r="K18" s="4"/>
@@ -5942,23 +5965,23 @@
       <c r="AB18" s="4"/>
     </row>
     <row r="19" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="39"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="23" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="42"/>
+        <v>0.25</v>
+      </c>
+      <c r="E19" s="36"/>
       <c r="F19" s="19">
-        <v>1</v>
-      </c>
-      <c r="G19" s="42"/>
+        <v>0.25</v>
+      </c>
+      <c r="G19" s="36"/>
       <c r="H19" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I19" s="5"/>
       <c r="K19" s="4"/>
@@ -5981,9 +6004,9 @@
       <c r="AB19" s="4"/>
     </row>
     <row r="20" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="39"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>24</v>
@@ -5991,13 +6014,13 @@
       <c r="D20" s="19">
         <v>1</v>
       </c>
-      <c r="E20" s="42"/>
+      <c r="E20" s="36"/>
       <c r="F20" s="19">
-        <v>1</v>
-      </c>
-      <c r="G20" s="42"/>
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="36"/>
       <c r="H20" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I20" s="5"/>
       <c r="K20" s="4"/>
@@ -6020,23 +6043,23 @@
       <c r="AB20" s="4"/>
     </row>
     <row r="21" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="39"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="23" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="19">
-        <v>0.25</v>
-      </c>
-      <c r="E21" s="42"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="36"/>
       <c r="F21" s="19">
-        <v>0.25</v>
-      </c>
-      <c r="G21" s="42"/>
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="36"/>
       <c r="H21" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I21" s="5"/>
       <c r="K21" s="4"/>
@@ -6059,7 +6082,7 @@
       <c r="AB21" s="4"/>
     </row>
     <row r="22" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="39"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="23" t="s">
         <v>90</v>
       </c>
@@ -6069,13 +6092,13 @@
       <c r="D22" s="19">
         <v>1</v>
       </c>
-      <c r="E22" s="42"/>
+      <c r="E22" s="36"/>
       <c r="F22" s="19">
         <v>0.5</v>
       </c>
-      <c r="G22" s="42"/>
+      <c r="G22" s="36"/>
       <c r="H22" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I22" s="5"/>
       <c r="K22" s="4"/>
@@ -6098,7 +6121,7 @@
       <c r="AB22" s="4"/>
     </row>
     <row r="23" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="39"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="23" t="s">
         <v>91</v>
       </c>
@@ -6106,15 +6129,15 @@
         <v>24</v>
       </c>
       <c r="D23" s="19">
-        <v>1</v>
-      </c>
-      <c r="E23" s="42"/>
+        <v>0.25</v>
+      </c>
+      <c r="E23" s="36"/>
       <c r="F23" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="G23" s="42"/>
+        <v>0.25</v>
+      </c>
+      <c r="G23" s="36"/>
       <c r="H23" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I23" s="5"/>
       <c r="K23" s="4"/>
@@ -6137,9 +6160,9 @@
       <c r="AB23" s="4"/>
     </row>
     <row r="24" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="39"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="23" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>24</v>
@@ -6147,13 +6170,13 @@
       <c r="D24" s="19">
         <v>1</v>
       </c>
-      <c r="E24" s="42"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="G24" s="42"/>
+        <v>0.75</v>
+      </c>
+      <c r="G24" s="36"/>
       <c r="H24" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I24" s="5"/>
       <c r="K24" s="4"/>
@@ -6176,23 +6199,23 @@
       <c r="AB24" s="4"/>
     </row>
     <row r="25" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="39"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="23" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="19">
-        <v>0.25</v>
-      </c>
-      <c r="E25" s="42"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="36"/>
       <c r="F25" s="19">
-        <v>0.25</v>
-      </c>
-      <c r="G25" s="42"/>
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="36"/>
       <c r="H25" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I25" s="5"/>
       <c r="K25" s="4"/>
@@ -6215,23 +6238,23 @@
       <c r="AB25" s="4"/>
     </row>
     <row r="26" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="39"/>
-      <c r="B26" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>22</v>
+      <c r="A26" s="34"/>
+      <c r="B26" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="D26" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="E26" s="42"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="36"/>
       <c r="F26" s="19">
         <v>0.5</v>
       </c>
-      <c r="G26" s="42"/>
+      <c r="G26" s="36"/>
       <c r="H26" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I26" s="5"/>
       <c r="K26" s="4"/>
@@ -6254,23 +6277,23 @@
       <c r="AB26" s="4"/>
     </row>
     <row r="27" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="39"/>
-      <c r="B27" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>22</v>
+      <c r="A27" s="34"/>
+      <c r="B27" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="D27" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="E27" s="42"/>
+        <v>0.25</v>
+      </c>
+      <c r="E27" s="36"/>
       <c r="F27" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="G27" s="42"/>
+        <v>0.25</v>
+      </c>
+      <c r="G27" s="36"/>
       <c r="H27" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I27" s="5"/>
       <c r="K27" s="4"/>
@@ -6293,23 +6316,17 @@
       <c r="AB27" s="4"/>
     </row>
     <row r="28" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="39"/>
-      <c r="B28" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="E28" s="42"/>
-      <c r="F28" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="G28" s="42"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="26"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="36"/>
       <c r="H28" s="30" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="I28" s="5"/>
       <c r="K28" s="4"/>
@@ -6332,23 +6349,17 @@
       <c r="AB28" s="4"/>
     </row>
     <row r="29" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="39"/>
-      <c r="B29" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="E29" s="42"/>
-      <c r="F29" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="G29" s="42"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="26"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="36"/>
       <c r="H29" s="30" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="I29" s="5"/>
       <c r="K29" s="4"/>
@@ -6371,23 +6382,17 @@
       <c r="AB29" s="4"/>
     </row>
     <row r="30" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="39"/>
-      <c r="B30" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="E30" s="42"/>
-      <c r="F30" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="G30" s="42"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="36"/>
       <c r="H30" s="30" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="I30" s="5"/>
       <c r="K30" s="4"/>
@@ -6410,23 +6415,17 @@
       <c r="AB30" s="4"/>
     </row>
     <row r="31" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="39"/>
-      <c r="B31" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="E31" s="42"/>
-      <c r="F31" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="G31" s="42"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="36"/>
       <c r="H31" s="30" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="I31" s="5"/>
       <c r="K31" s="4"/>
@@ -6449,9 +6448,9 @@
       <c r="AB31" s="4"/>
     </row>
     <row r="32" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="39"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="21" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C32" s="19" t="s">
         <v>22</v>
@@ -6459,13 +6458,13 @@
       <c r="D32" s="19">
         <v>0.75</v>
       </c>
-      <c r="E32" s="42"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="19">
         <v>0.5</v>
       </c>
-      <c r="G32" s="42"/>
+      <c r="G32" s="36"/>
       <c r="H32" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I32" s="5"/>
       <c r="K32" s="4"/>
@@ -6488,17 +6487,23 @@
       <c r="AB32" s="4"/>
     </row>
     <row r="33" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="39"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="42"/>
+        <v>58</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="E33" s="36"/>
+      <c r="F33" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="36"/>
       <c r="H33" s="30" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="I33" s="5"/>
       <c r="K33" s="4"/>
@@ -6521,17 +6526,23 @@
       <c r="AB33" s="4"/>
     </row>
     <row r="34" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="39"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="42"/>
+        <v>59</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="E34" s="36"/>
+      <c r="F34" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="36"/>
       <c r="H34" s="30" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="I34" s="5"/>
       <c r="K34" s="4"/>
@@ -6554,17 +6565,23 @@
       <c r="AB34" s="4"/>
     </row>
     <row r="35" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="40"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="43"/>
+        <v>60</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="E35" s="36"/>
+      <c r="F35" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="36"/>
       <c r="H35" s="30" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="I35" s="5"/>
       <c r="K35" s="4"/>
@@ -6587,31 +6604,23 @@
       <c r="AB35" s="4"/>
     </row>
     <row r="36" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="38" t="s">
-        <v>95</v>
-      </c>
+      <c r="A36" s="34"/>
       <c r="B36" s="21" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C36" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D36" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="E36" s="41">
-        <f>SUM(D36:D38)</f>
-        <v>4.5</v>
-      </c>
+        <v>0.75</v>
+      </c>
+      <c r="E36" s="36"/>
       <c r="F36" s="19">
-        <v>2</v>
-      </c>
-      <c r="G36" s="41">
-        <f>SUM(F36:F38)</f>
-        <v>5</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="36"/>
       <c r="H36" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I36" s="5"/>
       <c r="K36" s="4"/>
@@ -6634,23 +6643,23 @@
       <c r="AB36" s="4"/>
     </row>
     <row r="37" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="39"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="21" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C37" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="19">
-        <v>2</v>
-      </c>
-      <c r="E37" s="42"/>
+        <v>0.75</v>
+      </c>
+      <c r="E37" s="36"/>
       <c r="F37" s="19">
-        <v>2</v>
-      </c>
-      <c r="G37" s="42"/>
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="36"/>
       <c r="H37" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I37" s="5"/>
       <c r="K37" s="4"/>
@@ -6673,23 +6682,23 @@
       <c r="AB37" s="4"/>
     </row>
     <row r="38" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="40"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="21" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="C38" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D38" s="19">
-        <v>1</v>
-      </c>
-      <c r="E38" s="43"/>
+        <v>0.75</v>
+      </c>
+      <c r="E38" s="36"/>
       <c r="F38" s="19">
-        <v>1</v>
-      </c>
-      <c r="G38" s="43"/>
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="36"/>
       <c r="H38" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I38" s="5"/>
       <c r="K38" s="4"/>
@@ -6712,34 +6721,19 @@
       <c r="AB38" s="4"/>
     </row>
     <row r="39" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="19">
-        <v>2</v>
-      </c>
-      <c r="E39" s="41">
-        <f>SUM(D39:D42)</f>
-        <v>8</v>
-      </c>
-      <c r="F39" s="19">
-        <v>2</v>
-      </c>
-      <c r="G39" s="41">
-        <f>SUM(F39:F42)</f>
-        <v>9</v>
-      </c>
+      <c r="A39" s="34"/>
+      <c r="B39" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="36"/>
       <c r="H39" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="I39" s="5"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -6750,28 +6744,29 @@
       <c r="R39" s="4"/>
       <c r="S39" s="4"/>
       <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="4"/>
+      <c r="AA39" s="4"/>
+      <c r="AB39" s="4"/>
     </row>
     <row r="40" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="39"/>
-      <c r="B40" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="19">
-        <v>2</v>
-      </c>
-      <c r="E40" s="42"/>
-      <c r="F40" s="19">
-        <v>3</v>
-      </c>
-      <c r="G40" s="42"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="36"/>
       <c r="H40" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="I40" s="5"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -6782,28 +6777,29 @@
       <c r="R40" s="4"/>
       <c r="S40" s="4"/>
       <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+      <c r="W40" s="4"/>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4"/>
+      <c r="Z40" s="4"/>
+      <c r="AA40" s="4"/>
+      <c r="AB40" s="4"/>
     </row>
     <row r="41" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="39"/>
       <c r="B41" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="19">
-        <v>3</v>
-      </c>
-      <c r="E41" s="42"/>
-      <c r="F41" s="19">
-        <v>3</v>
-      </c>
-      <c r="G41" s="42"/>
+        <v>64</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="37"/>
       <c r="H41" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="I41" s="5"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -6814,28 +6810,43 @@
       <c r="R41" s="4"/>
       <c r="S41" s="4"/>
       <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
+      <c r="Z41" s="4"/>
+      <c r="AA41" s="4"/>
+      <c r="AB41" s="4"/>
     </row>
     <row r="42" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="39"/>
+      <c r="A42" s="33" t="s">
+        <v>93</v>
+      </c>
       <c r="B42" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D42" s="19">
-        <v>1</v>
-      </c>
-      <c r="E42" s="43"/>
+        <v>1.5</v>
+      </c>
+      <c r="E42" s="35">
+        <f>SUM(D42:D44)</f>
+        <v>4.5</v>
+      </c>
       <c r="F42" s="19">
-        <v>1</v>
-      </c>
-      <c r="G42" s="43"/>
+        <v>2</v>
+      </c>
+      <c r="G42" s="35">
+        <f>SUM(F42:F44)</f>
+        <v>5</v>
+      </c>
       <c r="H42" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="I42" s="5"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
@@ -6846,17 +6857,35 @@
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
       <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="4"/>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4"/>
+      <c r="AB42" s="4"/>
     </row>
     <row r="43" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="5"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="19">
+        <v>2</v>
+      </c>
+      <c r="E43" s="36"/>
+      <c r="F43" s="19">
+        <v>2</v>
+      </c>
+      <c r="G43" s="36"/>
+      <c r="H43" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="I43" s="5"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
@@ -6867,17 +6896,35 @@
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
       <c r="T43" s="4"/>
-    </row>
-    <row r="44" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="5"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4"/>
+      <c r="AB43" s="4"/>
+    </row>
+    <row r="44" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="39"/>
+      <c r="B44" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="19">
+        <v>1</v>
+      </c>
+      <c r="E44" s="37"/>
+      <c r="F44" s="19">
+        <v>1</v>
+      </c>
+      <c r="G44" s="37"/>
+      <c r="H44" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="I44" s="5"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
@@ -6888,15 +6935,42 @@
       <c r="R44" s="4"/>
       <c r="S44" s="4"/>
       <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="4"/>
+      <c r="Y44" s="4"/>
+      <c r="Z44" s="4"/>
+      <c r="AA44" s="4"/>
+      <c r="AB44" s="4"/>
     </row>
     <row r="45" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
+      <c r="A45" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="19">
+        <v>2</v>
+      </c>
+      <c r="E45" s="35">
+        <f>SUM(D45:D48)</f>
+        <v>8</v>
+      </c>
+      <c r="F45" s="19">
+        <v>2</v>
+      </c>
+      <c r="G45" s="35">
+        <f>SUM(F45:F48)</f>
+        <v>9</v>
+      </c>
+      <c r="H45" s="30" t="s">
+        <v>78</v>
+      </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -6911,12 +6985,24 @@
       <c r="T45" s="4"/>
     </row>
     <row r="46" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="19">
+        <v>2</v>
+      </c>
+      <c r="E46" s="36"/>
+      <c r="F46" s="19">
+        <v>3</v>
+      </c>
+      <c r="G46" s="36"/>
+      <c r="H46" s="30" t="s">
+        <v>78</v>
+      </c>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -6931,12 +7017,24 @@
       <c r="T46" s="4"/>
     </row>
     <row r="47" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="19">
+        <v>3</v>
+      </c>
+      <c r="E47" s="36"/>
+      <c r="F47" s="19">
+        <v>3</v>
+      </c>
+      <c r="G47" s="36"/>
+      <c r="H47" s="30" t="s">
+        <v>78</v>
+      </c>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -6951,12 +7049,24 @@
       <c r="T47" s="4"/>
     </row>
     <row r="48" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="19">
+        <v>1</v>
+      </c>
+      <c r="E48" s="37"/>
+      <c r="F48" s="19">
+        <v>1</v>
+      </c>
+      <c r="G48" s="37"/>
+      <c r="H48" s="30" t="s">
+        <v>78</v>
+      </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -6971,8 +7081,7 @@
       <c r="T48" s="4"/>
     </row>
     <row r="49" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
+      <c r="A49" s="5"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -6992,9 +7101,8 @@
       <c r="S49" s="4"/>
       <c r="T49" s="4"/>
     </row>
-    <row r="50" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+    <row r="50" spans="1:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -7015,8 +7123,7 @@
       <c r="T50" s="4"/>
     </row>
     <row r="51" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
+      <c r="A51" s="5"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -7036,11 +7143,144 @@
       <c r="S51" s="4"/>
       <c r="T51" s="4"/>
     </row>
+    <row r="52" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+    </row>
+    <row r="53" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="4"/>
+    </row>
+    <row r="54" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+    </row>
+    <row r="55" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+    </row>
+    <row r="56" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+    </row>
+    <row r="57" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="G45:G48"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -7048,19 +7288,12 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:H3"/>
-    <mergeCell ref="A12:A35"/>
-    <mergeCell ref="E12:E35"/>
-    <mergeCell ref="G12:G35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="G36:G38"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="A12:A41"/>
+    <mergeCell ref="E12:E41"/>
+    <mergeCell ref="G12:G41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="G42:G44"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:I6">
     <cfRule type="expression" dxfId="127" priority="2">
@@ -7082,7 +7315,7 @@
   </sheetPr>
   <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
@@ -7105,20 +7338,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -7177,40 +7410,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="45">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="G3" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="H3" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="I3" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="J3" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="46" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -7222,18 +7455,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -7248,35 +7481,35 @@
       </c>
       <c r="B5" s="11">
         <f>SUM('Sprint Backlog'!D:D)</f>
-        <v>44.25</v>
+        <v>47.5</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>38.71875</v>
+        <v>41.5625</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="1"/>
-        <v>33.1875</v>
+        <v>35.625</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>27.65625</v>
+        <v>29.6875</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="1"/>
-        <v>22.125</v>
+        <v>23.75</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="1"/>
-        <v>16.59375</v>
+        <v>17.8125</v>
       </c>
       <c r="H5" s="12">
         <f t="shared" si="1"/>
-        <v>11.0625</v>
+        <v>11.875</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" si="1"/>
-        <v>5.53125</v>
+        <v>5.9375</v>
       </c>
       <c r="J5" s="12">
         <f t="shared" si="1"/>
@@ -7284,11 +7517,11 @@
       </c>
       <c r="K5" s="12">
         <f>SUM(C5:J5)</f>
-        <v>154.875</v>
+        <v>166.25</v>
       </c>
       <c r="L5" s="12">
         <f>K5/A$3</f>
-        <v>19.359375</v>
+        <v>20.78125</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -7304,47 +7537,47 @@
       </c>
       <c r="B6" s="11">
         <f>B5</f>
-        <v>44.25</v>
+        <v>47.5</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>43.25</v>
+        <v>46.5</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="2"/>
-        <v>38.75</v>
+        <v>42</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="2"/>
-        <v>33.75</v>
+        <v>37</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="2"/>
-        <v>28.25</v>
+        <v>31.5</v>
       </c>
       <c r="G6" s="12">
         <f t="shared" si="2"/>
-        <v>26.75</v>
+        <v>30</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="2"/>
-        <v>20.75</v>
+        <v>24</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="2"/>
-        <v>17.75</v>
+        <v>21</v>
       </c>
       <c r="J6" s="12">
         <f t="shared" si="2"/>
-        <v>16.75</v>
+        <v>20</v>
       </c>
       <c r="K6" s="12">
         <f>SUM(C6:J6)</f>
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="L6" s="12">
         <f>K6/A$3</f>
-        <v>28.25</v>
+        <v>31.5</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -7382,18 +7615,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -7408,7 +7641,7 @@
       </c>
       <c r="B9" s="15">
         <f>B5/A3</f>
-        <v>5.53125</v>
+        <v>5.9375</v>
       </c>
       <c r="C9" s="15">
         <f t="shared" ref="C9:K9" si="3">SUM(C10:C12)</f>
@@ -7562,7 +7795,7 @@
       </c>
       <c r="B12" s="17">
         <f>Izaquiel!B9</f>
-        <v>1.5625</v>
+        <v>1.96875</v>
       </c>
       <c r="C12" s="12">
         <f>Izaquiel!C9</f>
@@ -8133,20 +8366,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -8205,40 +8438,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="45">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="G3" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="H3" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="I3" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="J3" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="46" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -8250,18 +8483,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -8410,18 +8643,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -8487,10 +8720,10 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="56"/>
+      <c r="A10" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="58"/>
       <c r="C10" s="12">
         <v>1</v>
       </c>
@@ -8524,18 +8757,18 @@
         <v>0.125</v>
       </c>
       <c r="M10" s="6"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="56"/>
+      <c r="A11" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="58"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -8569,18 +8802,18 @@
         <v>0.125</v>
       </c>
       <c r="M11" s="6"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="54"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="53"/>
+      <c r="A12" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="52"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -8614,18 +8847,18 @@
         <v>0.1875</v>
       </c>
       <c r="M12" s="6"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="54"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="53"/>
+      <c r="A13" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="52"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -8667,10 +8900,10 @@
       <c r="S13" s="6"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="53"/>
+      <c r="A14" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="52"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -8712,10 +8945,10 @@
       <c r="S14" s="6"/>
     </row>
     <row r="15" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="59"/>
+      <c r="A15" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="54"/>
       <c r="C15" s="12">
         <v>0</v>
       </c>
@@ -8757,10 +8990,10 @@
       <c r="S15" s="6"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="59"/>
+      <c r="A16" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="54"/>
       <c r="C16" s="12">
         <v>0</v>
       </c>
@@ -8802,10 +9035,10 @@
       <c r="S16" s="6"/>
     </row>
     <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="59"/>
+      <c r="A17" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="54"/>
       <c r="C17" s="12">
         <v>0</v>
       </c>
@@ -8847,10 +9080,10 @@
       <c r="S17" s="6"/>
     </row>
     <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="53"/>
+      <c r="A18" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="52"/>
       <c r="C18" s="12">
         <v>0</v>
       </c>
@@ -8892,10 +9125,10 @@
       <c r="S18" s="6"/>
     </row>
     <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="53"/>
+      <c r="A19" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="52"/>
       <c r="C19" s="12">
         <v>0</v>
       </c>
@@ -8937,10 +9170,10 @@
       <c r="S19" s="6"/>
     </row>
     <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="53"/>
+      <c r="A20" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="52"/>
       <c r="C20" s="12">
         <v>0</v>
       </c>
@@ -8980,10 +9213,10 @@
       <c r="Q20" s="6"/>
     </row>
     <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="53"/>
+      <c r="A21" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="52"/>
       <c r="C21" s="12">
         <v>0</v>
       </c>
@@ -9025,10 +9258,10 @@
       <c r="S21" s="6"/>
     </row>
     <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="52" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="53"/>
+      <c r="A22" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="52"/>
       <c r="C22" s="12">
         <v>0</v>
       </c>
@@ -9070,10 +9303,10 @@
       <c r="S22" s="6"/>
     </row>
     <row r="23" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="B23" s="53"/>
+      <c r="A23" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="52"/>
       <c r="C23" s="12">
         <v>0</v>
       </c>
@@ -9108,10 +9341,10 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="53"/>
+      <c r="A24" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="52"/>
       <c r="C24" s="12">
         <v>0</v>
       </c>
@@ -9146,10 +9379,10 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="53"/>
+      <c r="A25" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="52"/>
       <c r="C25" s="12">
         <v>0</v>
       </c>
@@ -9184,10 +9417,10 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" s="53"/>
+      <c r="A26" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="52"/>
       <c r="C26" s="12">
         <v>0</v>
       </c>
@@ -9222,10 +9455,10 @@
       </c>
     </row>
     <row r="27" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="53"/>
+      <c r="A27" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="52"/>
       <c r="C27" s="12">
         <v>0</v>
       </c>
@@ -9261,6 +9494,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
@@ -9277,26 +9530,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <conditionalFormatting sqref="N10:O19 N21:O22 M20 C10:L102">
     <cfRule type="expression" dxfId="29" priority="2">
@@ -9350,20 +9583,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -9422,40 +9655,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="45">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="46" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -9467,18 +9700,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -9493,35 +9726,35 @@
       </c>
       <c r="B5" s="11">
         <f>SUMIF('Sprint Backlog'!C:C,"=Izaquiel",'Sprint Backlog'!D:D)</f>
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>10.9375</v>
+        <v>13.78125</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="1"/>
-        <v>9.375</v>
+        <v>11.8125</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>7.8125</v>
+        <v>9.84375</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="1"/>
-        <v>6.25</v>
+        <v>7.875</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="1"/>
-        <v>4.6875</v>
+        <v>5.90625</v>
       </c>
       <c r="H5" s="12">
         <f t="shared" si="1"/>
-        <v>3.125</v>
+        <v>3.9375</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" si="1"/>
-        <v>1.5625</v>
+        <v>1.96875</v>
       </c>
       <c r="J5" s="12">
         <f t="shared" si="1"/>
@@ -9529,11 +9762,11 @@
       </c>
       <c r="K5" s="12">
         <f>SUM(C5:J5)</f>
-        <v>43.75</v>
+        <v>55.125</v>
       </c>
       <c r="L5" s="12">
         <f>K5/A$3</f>
-        <v>5.46875</v>
+        <v>6.890625</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -9549,47 +9782,47 @@
       </c>
       <c r="B6" s="11">
         <f>B5</f>
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c r="G6" s="12">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c r="J6" s="12">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c r="K6" s="12">
         <f>SUM(C6:J6)</f>
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="L6" s="12">
         <f>K6/A$3</f>
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -9627,18 +9860,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -9653,7 +9886,7 @@
       </c>
       <c r="B9" s="15">
         <f>B5/A3</f>
-        <v>1.5625</v>
+        <v>1.96875</v>
       </c>
       <c r="C9" s="15">
         <f>SUM(C10:C32)</f>
@@ -9704,10 +9937,10 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="63"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="12">
         <v>0</v>
       </c>
@@ -9749,10 +9982,10 @@
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="63"/>
+      <c r="B11" s="62"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -9794,10 +10027,10 @@
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="65"/>
+      <c r="B12" s="64"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -9839,10 +10072,10 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="65"/>
+      <c r="B13" s="64"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -9877,10 +10110,10 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="61"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -9915,10 +10148,10 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="61"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="12">
         <v>0</v>
       </c>
@@ -9953,10 +10186,10 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="61"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="12">
         <v>0</v>
       </c>
@@ -9991,10 +10224,10 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="61"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="12">
         <v>0</v>
       </c>
@@ -10032,6 +10265,14 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
@@ -10047,14 +10288,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:L98 K10:L10 A14:A17">
     <cfRule type="expression" dxfId="24" priority="17">
@@ -10154,20 +10387,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -10226,40 +10459,40 @@
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="45">
         <v>8</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="G3" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="H3" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="I3" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="J3" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="46" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="6"/>
@@ -10271,18 +10504,18 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -10431,18 +10664,18 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -10508,10 +10741,10 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="63"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="12">
         <v>0</v>
       </c>
@@ -10553,10 +10786,10 @@
       <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="63"/>
+      <c r="B11" s="62"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -10598,10 +10831,10 @@
       <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="63"/>
+      <c r="B12" s="62"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -10643,10 +10876,10 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="61"/>
+      <c r="A13" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="60"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -10686,6 +10919,10 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C1:L1"/>
@@ -10701,10 +10938,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:L96">
     <cfRule type="expression" dxfId="9" priority="19">

</xml_diff>